<commit_message>
added minutes folder and barchart
</commit_message>
<xml_diff>
--- a/run_plan.xlsx
+++ b/run_plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukes\Dissertation\Parallel-PSO-OPF-Scalability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7A3B27-1440-477E-9955-D86BA39427EC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E301EEF-4838-464C-AA97-E4966E2A152A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="serialRuns" sheetId="1" r:id="rId1"/>
@@ -105,10 +105,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,7 +391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -403,22 +403,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f>"serial-particles"&amp;B2&amp;"-run"&amp;D2</f>
+        <f t="shared" ref="A2:A19" si="0">"serial-particles"&amp;B2&amp;"-run"&amp;D2</f>
         <v>serial-particles20-run1</v>
       </c>
       <c r="B2">
@@ -433,7 +433,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f>"serial-particles"&amp;B3&amp;"-run"&amp;D3</f>
+        <f t="shared" si="0"/>
         <v>serial-particles20-run2</v>
       </c>
       <c r="B3">
@@ -448,7 +448,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>"serial-particles"&amp;B4&amp;"-run"&amp;D4</f>
+        <f t="shared" si="0"/>
         <v>serial-particles20-run3</v>
       </c>
       <c r="B4">
@@ -463,7 +463,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f>"serial-particles"&amp;B5&amp;"-run"&amp;D5</f>
+        <f t="shared" si="0"/>
         <v>serial-particles60-run1</v>
       </c>
       <c r="B5">
@@ -478,7 +478,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f>"serial-particles"&amp;B6&amp;"-run"&amp;D6</f>
+        <f t="shared" si="0"/>
         <v>serial-particles60-run2</v>
       </c>
       <c r="B6">
@@ -493,7 +493,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f>"serial-particles"&amp;B7&amp;"-run"&amp;D7</f>
+        <f t="shared" si="0"/>
         <v>serial-particles60-run3</v>
       </c>
       <c r="B7">
@@ -508,7 +508,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f>"serial-particles"&amp;B8&amp;"-run"&amp;D8</f>
+        <f t="shared" si="0"/>
         <v>serial-particles100-run1</v>
       </c>
       <c r="B8">
@@ -523,7 +523,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f>"serial-particles"&amp;B9&amp;"-run"&amp;D9</f>
+        <f t="shared" si="0"/>
         <v>serial-particles100-run2</v>
       </c>
       <c r="B9">
@@ -538,7 +538,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f>"serial-particles"&amp;B10&amp;"-run"&amp;D10</f>
+        <f t="shared" si="0"/>
         <v>serial-particles100-run3</v>
       </c>
       <c r="B10">
@@ -553,7 +553,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>"serial-particles"&amp;B11&amp;"-run"&amp;D11</f>
+        <f t="shared" si="0"/>
         <v>serial-particles140-run1</v>
       </c>
       <c r="B11">
@@ -568,7 +568,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>"serial-particles"&amp;B12&amp;"-run"&amp;D12</f>
+        <f t="shared" si="0"/>
         <v>serial-particles140-run2</v>
       </c>
       <c r="B12">
@@ -583,7 +583,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>"serial-particles"&amp;B13&amp;"-run"&amp;D13</f>
+        <f t="shared" si="0"/>
         <v>serial-particles140-run3</v>
       </c>
       <c r="B13">
@@ -598,7 +598,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f>"serial-particles"&amp;B14&amp;"-run"&amp;D14</f>
+        <f t="shared" si="0"/>
         <v>serial-particles180-run1</v>
       </c>
       <c r="B14">
@@ -613,7 +613,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f>"serial-particles"&amp;B15&amp;"-run"&amp;D15</f>
+        <f t="shared" si="0"/>
         <v>serial-particles180-run2</v>
       </c>
       <c r="B15">
@@ -628,7 +628,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f>"serial-particles"&amp;B16&amp;"-run"&amp;D16</f>
+        <f t="shared" si="0"/>
         <v>serial-particles180-run3</v>
       </c>
       <c r="B16">
@@ -643,7 +643,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f>"serial-particles"&amp;B17&amp;"-run"&amp;D17</f>
+        <f t="shared" si="0"/>
         <v>serial-particles220-run1</v>
       </c>
       <c r="B17">
@@ -658,7 +658,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f>"serial-particles"&amp;B18&amp;"-run"&amp;D18</f>
+        <f t="shared" si="0"/>
         <v>serial-particles220-run2</v>
       </c>
       <c r="B18">
@@ -673,7 +673,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f>"serial-particles"&amp;B19&amp;"-run"&amp;D19</f>
+        <f t="shared" si="0"/>
         <v>serial-particles220-run3</v>
       </c>
       <c r="B19">
@@ -696,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1102CE02-4A00-4625-A7BD-467D2E2DB84D}">
   <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -706,13 +706,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -885,19 +885,19 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -958,16 +958,16 @@
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
         <f>"parallel-particles"&amp;B15&amp;"-threads"&amp;D15&amp;"-run"&amp;E15</f>
-        <v>parallel-particles60-threads12-run1</v>
+        <v>parallel-particles20-threads16-run1</v>
       </c>
       <c r="B15">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
       </c>
       <c r="D15">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -976,7 +976,7 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
         <f>"parallel-particles"&amp;B16&amp;"-threads"&amp;D16&amp;"-run"&amp;E16</f>
-        <v>parallel-particles20-threads16-run1</v>
+        <v>parallel-particles20-threads20-run1</v>
       </c>
       <c r="B16">
         <v>20</v>
@@ -985,7 +985,7 @@
         <v>6</v>
       </c>
       <c r="D16">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -994,16 +994,16 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
         <f>"parallel-particles"&amp;B17&amp;"-threads"&amp;D17&amp;"-run"&amp;E17</f>
-        <v>parallel-particles20-threads20-run1</v>
+        <v>parallel-particles60-threads12-run1</v>
       </c>
       <c r="B17">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
         <v>6</v>
       </c>
       <c r="D17">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E17">
         <v>1</v>
@@ -1012,16 +1012,16 @@
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
         <f>"parallel-particles"&amp;B18&amp;"-threads"&amp;D18&amp;"-run"&amp;E18</f>
-        <v>parallel-particles100-threads20-run1</v>
+        <v>parallel-particles60-threads24-run1</v>
       </c>
       <c r="B18">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
       </c>
       <c r="D18">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -1030,7 +1030,7 @@
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
         <f>"parallel-particles"&amp;B19&amp;"-threads"&amp;D19&amp;"-run"&amp;E19</f>
-        <v>parallel-particles60-threads24-run1</v>
+        <v>parallel-particles60-threads36-run1</v>
       </c>
       <c r="B19">
         <v>60</v>
@@ -1039,7 +1039,7 @@
         <v>6</v>
       </c>
       <c r="D19">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="E19">
         <v>1</v>
@@ -1048,16 +1048,16 @@
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
         <f>"parallel-particles"&amp;B20&amp;"-threads"&amp;D20&amp;"-run"&amp;E20</f>
-        <v>parallel-particles140-threads28-run1</v>
+        <v>parallel-particles60-threads48-run1</v>
       </c>
       <c r="B20">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="C20" t="s">
         <v>6</v>
       </c>
       <c r="D20">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -1066,7 +1066,7 @@
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
         <f>"parallel-particles"&amp;B21&amp;"-threads"&amp;D21&amp;"-run"&amp;E21</f>
-        <v>parallel-particles60-threads36-run1</v>
+        <v>parallel-particles60-threads60-run1</v>
       </c>
       <c r="B21">
         <v>60</v>
@@ -1075,7 +1075,7 @@
         <v>6</v>
       </c>
       <c r="D21">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -1084,16 +1084,16 @@
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
         <f>"parallel-particles"&amp;B22&amp;"-threads"&amp;D22&amp;"-run"&amp;E22</f>
-        <v>parallel-particles180-threads36-run1</v>
+        <v>parallel-particles100-threads20-run1</v>
       </c>
       <c r="B22">
-        <v>180</v>
+        <v>100</v>
       </c>
       <c r="C22" t="s">
         <v>6</v>
       </c>
       <c r="D22">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E22">
         <v>1</v>
@@ -1120,16 +1120,16 @@
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
         <f>"parallel-particles"&amp;B24&amp;"-threads"&amp;D24&amp;"-run"&amp;E24</f>
-        <v>parallel-particles220-threads44-run1</v>
+        <v>parallel-particles100-threads60-run1</v>
       </c>
       <c r="B24">
-        <v>220</v>
+        <v>100</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
       </c>
       <c r="D24">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -1138,16 +1138,16 @@
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
         <f>"parallel-particles"&amp;B25&amp;"-threads"&amp;D25&amp;"-run"&amp;E25</f>
-        <v>parallel-particles60-threads48-run1</v>
+        <v>parallel-particles100-threads80-run1</v>
       </c>
       <c r="B25">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
       </c>
       <c r="D25">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="E25">
         <v>1</v>
@@ -1156,16 +1156,16 @@
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
         <f>"parallel-particles"&amp;B26&amp;"-threads"&amp;D26&amp;"-run"&amp;E26</f>
-        <v>parallel-particles140-threads56-run1</v>
+        <v>parallel-particles100-threads100-run1</v>
       </c>
       <c r="B26">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
       </c>
       <c r="D26">
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -1174,16 +1174,16 @@
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
         <f>"parallel-particles"&amp;B27&amp;"-threads"&amp;D27&amp;"-run"&amp;E27</f>
-        <v>parallel-particles60-threads60-run1</v>
+        <v>parallel-particles140-threads28-run1</v>
       </c>
       <c r="B27">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
       </c>
       <c r="D27">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="E27">
         <v>1</v>
@@ -1192,16 +1192,16 @@
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
         <f>"parallel-particles"&amp;B28&amp;"-threads"&amp;D28&amp;"-run"&amp;E28</f>
-        <v>parallel-particles100-threads60-run1</v>
+        <v>parallel-particles140-threads56-run1</v>
       </c>
       <c r="B28">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
       </c>
       <c r="D28">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E28">
         <v>1</v>
@@ -1210,16 +1210,16 @@
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
         <f>"parallel-particles"&amp;B29&amp;"-threads"&amp;D29&amp;"-run"&amp;E29</f>
-        <v>parallel-particles180-threads72-run1</v>
+        <v>parallel-particles140-threads84-run1</v>
       </c>
       <c r="B29">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
       </c>
       <c r="D29">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="E29">
         <v>1</v>
@@ -1228,16 +1228,16 @@
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
         <f>"parallel-particles"&amp;B30&amp;"-threads"&amp;D30&amp;"-run"&amp;E30</f>
-        <v>parallel-particles100-threads80-run1</v>
+        <v>parallel-particles140-threads112-run1</v>
       </c>
       <c r="B30">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
       </c>
       <c r="D30">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1246,7 +1246,7 @@
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
         <f>"parallel-particles"&amp;B31&amp;"-threads"&amp;D31&amp;"-run"&amp;E31</f>
-        <v>parallel-particles140-threads84-run1</v>
+        <v>parallel-particles140-threads140-run1</v>
       </c>
       <c r="B31">
         <v>140</v>
@@ -1255,7 +1255,7 @@
         <v>6</v>
       </c>
       <c r="D31">
-        <v>84</v>
+        <v>140</v>
       </c>
       <c r="E31">
         <v>1</v>
@@ -1264,16 +1264,16 @@
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
         <f>"parallel-particles"&amp;B32&amp;"-threads"&amp;D32&amp;"-run"&amp;E32</f>
-        <v>parallel-particles220-threads88-run1</v>
+        <v>parallel-particles180-threads36-run1</v>
       </c>
       <c r="B32">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
       </c>
       <c r="D32">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="E32">
         <v>1</v>
@@ -1282,16 +1282,16 @@
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
         <f>"parallel-particles"&amp;B33&amp;"-threads"&amp;D33&amp;"-run"&amp;E33</f>
-        <v>parallel-particles100-threads100-run1</v>
+        <v>parallel-particles180-threads72-run1</v>
       </c>
       <c r="B33">
-        <v>100</v>
+        <v>180</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
       </c>
       <c r="D33">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="E33">
         <v>1</v>
@@ -1318,16 +1318,16 @@
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
         <f>"parallel-particles"&amp;B35&amp;"-threads"&amp;D35&amp;"-run"&amp;E35</f>
-        <v>parallel-particles140-threads112-run1</v>
+        <v>parallel-particles180-threads144-run1</v>
       </c>
       <c r="B35">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="C35" t="s">
         <v>6</v>
       </c>
       <c r="D35">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="E35">
         <v>1</v>
@@ -1336,16 +1336,16 @@
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
         <f>"parallel-particles"&amp;B36&amp;"-threads"&amp;D36&amp;"-run"&amp;E36</f>
-        <v>parallel-particles220-threads132-run1</v>
+        <v>parallel-particles180-threads180-run1</v>
       </c>
       <c r="B36">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
       </c>
       <c r="D36">
-        <v>132</v>
+        <v>180</v>
       </c>
       <c r="E36">
         <v>1</v>
@@ -1354,16 +1354,16 @@
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
         <f>"parallel-particles"&amp;B37&amp;"-threads"&amp;D37&amp;"-run"&amp;E37</f>
-        <v>parallel-particles140-threads140-run1</v>
+        <v>parallel-particles220-threads44-run1</v>
       </c>
       <c r="B37">
-        <v>140</v>
+        <v>220</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
       </c>
       <c r="D37">
-        <v>140</v>
+        <v>44</v>
       </c>
       <c r="E37">
         <v>1</v>
@@ -1372,16 +1372,16 @@
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
         <f>"parallel-particles"&amp;B38&amp;"-threads"&amp;D38&amp;"-run"&amp;E38</f>
-        <v>parallel-particles180-threads144-run1</v>
+        <v>parallel-particles220-threads88-run1</v>
       </c>
       <c r="B38">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="C38" t="s">
         <v>6</v>
       </c>
       <c r="D38">
-        <v>144</v>
+        <v>88</v>
       </c>
       <c r="E38">
         <v>1</v>
@@ -1390,7 +1390,7 @@
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
         <f>"parallel-particles"&amp;B39&amp;"-threads"&amp;D39&amp;"-run"&amp;E39</f>
-        <v>parallel-particles220-threads176-run1</v>
+        <v>parallel-particles220-threads132-run1</v>
       </c>
       <c r="B39">
         <v>220</v>
@@ -1399,7 +1399,7 @@
         <v>6</v>
       </c>
       <c r="D39">
-        <v>176</v>
+        <v>132</v>
       </c>
       <c r="E39">
         <v>1</v>
@@ -1408,16 +1408,16 @@
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
         <f>"parallel-particles"&amp;B40&amp;"-threads"&amp;D40&amp;"-run"&amp;E40</f>
-        <v>parallel-particles180-threads180-run1</v>
+        <v>parallel-particles220-threads176-run1</v>
       </c>
       <c r="B40">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
       </c>
       <c r="D40">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E40">
         <v>1</v>
@@ -1498,16 +1498,16 @@
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
         <f>"parallel-particles"&amp;B45&amp;"-threads"&amp;D45&amp;"-run"&amp;E45</f>
-        <v>parallel-particles60-threads12-run2</v>
+        <v>parallel-particles20-threads16-run2</v>
       </c>
       <c r="B45">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
       </c>
       <c r="D45">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E45">
         <v>2</v>
@@ -1516,7 +1516,7 @@
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
         <f>"parallel-particles"&amp;B46&amp;"-threads"&amp;D46&amp;"-run"&amp;E46</f>
-        <v>parallel-particles20-threads16-run2</v>
+        <v>parallel-particles20-threads20-run2</v>
       </c>
       <c r="B46">
         <v>20</v>
@@ -1525,7 +1525,7 @@
         <v>6</v>
       </c>
       <c r="D46">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E46">
         <v>2</v>
@@ -1534,16 +1534,16 @@
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
         <f>"parallel-particles"&amp;B47&amp;"-threads"&amp;D47&amp;"-run"&amp;E47</f>
-        <v>parallel-particles20-threads20-run2</v>
+        <v>parallel-particles60-threads12-run2</v>
       </c>
       <c r="B47">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C47" t="s">
         <v>6</v>
       </c>
       <c r="D47">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E47">
         <v>2</v>
@@ -1552,16 +1552,16 @@
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
         <f>"parallel-particles"&amp;B48&amp;"-threads"&amp;D48&amp;"-run"&amp;E48</f>
-        <v>parallel-particles100-threads20-run2</v>
+        <v>parallel-particles60-threads24-run2</v>
       </c>
       <c r="B48">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
       </c>
       <c r="D48">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E48">
         <v>2</v>
@@ -1570,7 +1570,7 @@
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
         <f>"parallel-particles"&amp;B49&amp;"-threads"&amp;D49&amp;"-run"&amp;E49</f>
-        <v>parallel-particles60-threads24-run2</v>
+        <v>parallel-particles60-threads36-run2</v>
       </c>
       <c r="B49">
         <v>60</v>
@@ -1579,7 +1579,7 @@
         <v>6</v>
       </c>
       <c r="D49">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="E49">
         <v>2</v>
@@ -1588,16 +1588,16 @@
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
         <f>"parallel-particles"&amp;B50&amp;"-threads"&amp;D50&amp;"-run"&amp;E50</f>
-        <v>parallel-particles140-threads28-run2</v>
+        <v>parallel-particles60-threads48-run2</v>
       </c>
       <c r="B50">
-        <v>140</v>
+        <v>60</v>
       </c>
       <c r="C50" t="s">
         <v>6</v>
       </c>
       <c r="D50">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="E50">
         <v>2</v>
@@ -1606,7 +1606,7 @@
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
         <f>"parallel-particles"&amp;B51&amp;"-threads"&amp;D51&amp;"-run"&amp;E51</f>
-        <v>parallel-particles60-threads36-run2</v>
+        <v>parallel-particles60-threads60-run2</v>
       </c>
       <c r="B51">
         <v>60</v>
@@ -1615,7 +1615,7 @@
         <v>6</v>
       </c>
       <c r="D51">
-        <v>36</v>
+        <v>60</v>
       </c>
       <c r="E51">
         <v>2</v>
@@ -1624,16 +1624,16 @@
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
         <f>"parallel-particles"&amp;B52&amp;"-threads"&amp;D52&amp;"-run"&amp;E52</f>
-        <v>parallel-particles180-threads36-run2</v>
+        <v>parallel-particles100-threads20-run2</v>
       </c>
       <c r="B52">
-        <v>180</v>
+        <v>100</v>
       </c>
       <c r="C52" t="s">
         <v>6</v>
       </c>
       <c r="D52">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="E52">
         <v>2</v>
@@ -1660,16 +1660,16 @@
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
         <f>"parallel-particles"&amp;B54&amp;"-threads"&amp;D54&amp;"-run"&amp;E54</f>
-        <v>parallel-particles220-threads44-run2</v>
+        <v>parallel-particles100-threads60-run2</v>
       </c>
       <c r="B54">
-        <v>220</v>
+        <v>100</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
       </c>
       <c r="D54">
-        <v>44</v>
+        <v>60</v>
       </c>
       <c r="E54">
         <v>2</v>
@@ -1678,16 +1678,16 @@
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
         <f>"parallel-particles"&amp;B55&amp;"-threads"&amp;D55&amp;"-run"&amp;E55</f>
-        <v>parallel-particles60-threads48-run2</v>
+        <v>parallel-particles100-threads80-run2</v>
       </c>
       <c r="B55">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
       </c>
       <c r="D55">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="E55">
         <v>2</v>
@@ -1696,16 +1696,16 @@
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
         <f>"parallel-particles"&amp;B56&amp;"-threads"&amp;D56&amp;"-run"&amp;E56</f>
-        <v>parallel-particles140-threads56-run2</v>
+        <v>parallel-particles100-threads100-run2</v>
       </c>
       <c r="B56">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
       </c>
       <c r="D56">
-        <v>56</v>
+        <v>100</v>
       </c>
       <c r="E56">
         <v>2</v>
@@ -1714,16 +1714,16 @@
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
         <f>"parallel-particles"&amp;B57&amp;"-threads"&amp;D57&amp;"-run"&amp;E57</f>
-        <v>parallel-particles60-threads60-run2</v>
+        <v>parallel-particles140-threads28-run2</v>
       </c>
       <c r="B57">
-        <v>60</v>
+        <v>140</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
       </c>
       <c r="D57">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="E57">
         <v>2</v>
@@ -1732,16 +1732,16 @@
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
         <f>"parallel-particles"&amp;B58&amp;"-threads"&amp;D58&amp;"-run"&amp;E58</f>
-        <v>parallel-particles100-threads60-run2</v>
+        <v>parallel-particles140-threads56-run2</v>
       </c>
       <c r="B58">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="C58" t="s">
         <v>6</v>
       </c>
       <c r="D58">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E58">
         <v>2</v>
@@ -1750,16 +1750,16 @@
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
         <f>"parallel-particles"&amp;B59&amp;"-threads"&amp;D59&amp;"-run"&amp;E59</f>
-        <v>parallel-particles180-threads72-run2</v>
+        <v>parallel-particles140-threads84-run2</v>
       </c>
       <c r="B59">
-        <v>180</v>
+        <v>140</v>
       </c>
       <c r="C59" t="s">
         <v>6</v>
       </c>
       <c r="D59">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="E59">
         <v>2</v>
@@ -1768,16 +1768,16 @@
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
         <f>"parallel-particles"&amp;B60&amp;"-threads"&amp;D60&amp;"-run"&amp;E60</f>
-        <v>parallel-particles100-threads80-run2</v>
+        <v>parallel-particles140-threads112-run2</v>
       </c>
       <c r="B60">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="C60" t="s">
         <v>6</v>
       </c>
       <c r="D60">
-        <v>80</v>
+        <v>112</v>
       </c>
       <c r="E60">
         <v>2</v>
@@ -1786,7 +1786,7 @@
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
         <f>"parallel-particles"&amp;B61&amp;"-threads"&amp;D61&amp;"-run"&amp;E61</f>
-        <v>parallel-particles140-threads84-run2</v>
+        <v>parallel-particles140-threads140-run2</v>
       </c>
       <c r="B61">
         <v>140</v>
@@ -1795,7 +1795,7 @@
         <v>6</v>
       </c>
       <c r="D61">
-        <v>84</v>
+        <v>140</v>
       </c>
       <c r="E61">
         <v>2</v>
@@ -1804,16 +1804,16 @@
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
         <f>"parallel-particles"&amp;B62&amp;"-threads"&amp;D62&amp;"-run"&amp;E62</f>
-        <v>parallel-particles220-threads88-run2</v>
+        <v>parallel-particles180-threads36-run2</v>
       </c>
       <c r="B62">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
       </c>
       <c r="D62">
-        <v>88</v>
+        <v>36</v>
       </c>
       <c r="E62">
         <v>2</v>
@@ -1822,16 +1822,16 @@
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
         <f>"parallel-particles"&amp;B63&amp;"-threads"&amp;D63&amp;"-run"&amp;E63</f>
-        <v>parallel-particles100-threads100-run2</v>
+        <v>parallel-particles180-threads72-run2</v>
       </c>
       <c r="B63">
-        <v>100</v>
+        <v>180</v>
       </c>
       <c r="C63" t="s">
         <v>6</v>
       </c>
       <c r="D63">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="E63">
         <v>2</v>
@@ -1858,16 +1858,16 @@
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
         <f>"parallel-particles"&amp;B65&amp;"-threads"&amp;D65&amp;"-run"&amp;E65</f>
-        <v>parallel-particles140-threads112-run2</v>
+        <v>parallel-particles180-threads144-run2</v>
       </c>
       <c r="B65">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="C65" t="s">
         <v>6</v>
       </c>
       <c r="D65">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="E65">
         <v>2</v>
@@ -1876,16 +1876,16 @@
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
         <f>"parallel-particles"&amp;B66&amp;"-threads"&amp;D66&amp;"-run"&amp;E66</f>
-        <v>parallel-particles220-threads132-run2</v>
+        <v>parallel-particles180-threads180-run2</v>
       </c>
       <c r="B66">
-        <v>220</v>
+        <v>180</v>
       </c>
       <c r="C66" t="s">
         <v>6</v>
       </c>
       <c r="D66">
-        <v>132</v>
+        <v>180</v>
       </c>
       <c r="E66">
         <v>2</v>
@@ -1894,16 +1894,16 @@
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f>"parallel-particles"&amp;B67&amp;"-threads"&amp;D67&amp;"-run"&amp;E67</f>
-        <v>parallel-particles140-threads140-run2</v>
+        <v>parallel-particles220-threads44-run2</v>
       </c>
       <c r="B67">
-        <v>140</v>
+        <v>220</v>
       </c>
       <c r="C67" t="s">
         <v>6</v>
       </c>
       <c r="D67">
-        <v>140</v>
+        <v>44</v>
       </c>
       <c r="E67">
         <v>2</v>
@@ -1912,16 +1912,16 @@
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
         <f>"parallel-particles"&amp;B68&amp;"-threads"&amp;D68&amp;"-run"&amp;E68</f>
-        <v>parallel-particles180-threads144-run2</v>
+        <v>parallel-particles220-threads88-run2</v>
       </c>
       <c r="B68">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="C68" t="s">
         <v>6</v>
       </c>
       <c r="D68">
-        <v>144</v>
+        <v>88</v>
       </c>
       <c r="E68">
         <v>2</v>
@@ -1930,7 +1930,7 @@
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
         <f>"parallel-particles"&amp;B69&amp;"-threads"&amp;D69&amp;"-run"&amp;E69</f>
-        <v>parallel-particles220-threads176-run2</v>
+        <v>parallel-particles220-threads132-run2</v>
       </c>
       <c r="B69">
         <v>220</v>
@@ -1939,7 +1939,7 @@
         <v>6</v>
       </c>
       <c r="D69">
-        <v>176</v>
+        <v>132</v>
       </c>
       <c r="E69">
         <v>2</v>
@@ -1948,16 +1948,16 @@
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
         <f>"parallel-particles"&amp;B70&amp;"-threads"&amp;D70&amp;"-run"&amp;E70</f>
-        <v>parallel-particles180-threads180-run2</v>
+        <v>parallel-particles220-threads176-run2</v>
       </c>
       <c r="B70">
-        <v>180</v>
+        <v>220</v>
       </c>
       <c r="C70" t="s">
         <v>6</v>
       </c>
       <c r="D70">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="E70">
         <v>2</v>
@@ -1983,8 +1983,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A11:E11" xr:uid="{F1014102-F14F-4AB9-959E-C9503DEB0969}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:E41">
-      <sortCondition ref="D11"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:E71">
+      <sortCondition ref="E11"/>
     </sortState>
   </autoFilter>
   <mergeCells count="1">

</xml_diff>

<commit_message>
implemented MPI, generated initial run results
</commit_message>
<xml_diff>
--- a/run_plan.xlsx
+++ b/run_plan.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukes\Dissertation\Parallel-PSO-OPF-Scalability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E301EEF-4838-464C-AA97-E4966E2A152A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE8B067-2502-4938-A2B6-1B4AA056E711}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31590" yWindow="705" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="serialRuns" sheetId="1" r:id="rId1"/>
     <sheet name="parallelRuns" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">parallelRuns!$A$11:$E$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">parallelRuns!$A$11:$E$71</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">serialRuns!$A$1:$D$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="8">
   <si>
     <t>run_name</t>
   </si>
@@ -50,9 +50,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>nThreads</t>
-  </si>
-  <si>
     <t>serial</t>
   </si>
   <si>
@@ -60,6 +57,12 @@
   </si>
   <si>
     <t>parallel</t>
+  </si>
+  <si>
+    <t>nProcesses</t>
+  </si>
+  <si>
+    <t>command</t>
   </si>
 </sst>
 </file>
@@ -413,7 +416,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -425,7 +428,7 @@
         <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -440,7 +443,7 @@
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -455,7 +458,7 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -470,7 +473,7 @@
         <v>60</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -485,7 +488,7 @@
         <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -500,7 +503,7 @@
         <v>60</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -515,7 +518,7 @@
         <v>100</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -530,7 +533,7 @@
         <v>100</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -545,7 +548,7 @@
         <v>100</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -560,7 +563,7 @@
         <v>140</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -575,7 +578,7 @@
         <v>140</v>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12">
         <v>2</v>
@@ -590,7 +593,7 @@
         <v>140</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -605,7 +608,7 @@
         <v>180</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -620,7 +623,7 @@
         <v>180</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -635,7 +638,7 @@
         <v>180</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16">
         <v>3</v>
@@ -650,7 +653,7 @@
         <v>220</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -665,7 +668,7 @@
         <v>220</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18">
         <v>2</v>
@@ -680,7 +683,7 @@
         <v>220</v>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D19">
         <v>3</v>
@@ -694,27 +697,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1102CE02-4A00-4625-A7BD-467D2E2DB84D}">
-  <dimension ref="A1:F71"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:G71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="100.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -734,7 +739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20</v>
       </c>
@@ -759,7 +764,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>60</v>
       </c>
@@ -784,7 +789,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>100</v>
       </c>
@@ -809,7 +814,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>140</v>
       </c>
@@ -834,7 +839,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>180</v>
       </c>
@@ -859,7 +864,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>220</v>
       </c>
@@ -884,7 +889,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
@@ -895,22 +900,25 @@
         <v>2</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>"parallel-particles"&amp;B12&amp;"-threads"&amp;D12&amp;"-run"&amp;E12</f>
-        <v>parallel-particles20-threads4-run1</v>
+        <f>"parallel_particles"&amp;B12&amp;"_processes"&amp;D12&amp;"_run"&amp;E12</f>
+        <v>parallel_particles20_processes4_run1</v>
       </c>
       <c r="B12">
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -918,17 +926,21 @@
       <c r="E12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="str">
+        <f>"srun python parallel_mpi_pso_algorithm.py "&amp;CHAR(34)&amp;CHAR(34) &amp;" 50 "&amp;B12&amp;" 0.25 0.2 0.7 "&amp;A12&amp;" "&amp;D12</f>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes4_run1 4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>"parallel-particles"&amp;B13&amp;"-threads"&amp;D13&amp;"-run"&amp;E13</f>
-        <v>parallel-particles20-threads8-run1</v>
+        <f t="shared" ref="A13:A71" si="2">"parallel_particles"&amp;B13&amp;"_processes"&amp;D13&amp;"_run"&amp;E13</f>
+        <v>parallel_particles20_processes8_run1</v>
       </c>
       <c r="B13">
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D13">
         <v>8</v>
@@ -936,17 +948,21 @@
       <c r="E13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="str">
+        <f t="shared" ref="G13:G71" si="3">"srun python parallel_mpi_pso_algorithm.py "&amp;CHAR(34)&amp;CHAR(34) &amp;" 50 "&amp;B13&amp;" 0.25 0.2 0.7 "&amp;A13&amp;" "&amp;D13</f>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes8_run1 8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f>"parallel-particles"&amp;B14&amp;"-threads"&amp;D14&amp;"-run"&amp;E14</f>
-        <v>parallel-particles20-threads12-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles20_processes12_run1</v>
       </c>
       <c r="B14">
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D14">
         <v>12</v>
@@ -954,17 +970,21 @@
       <c r="E14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes12_run1 12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f>"parallel-particles"&amp;B15&amp;"-threads"&amp;D15&amp;"-run"&amp;E15</f>
-        <v>parallel-particles20-threads16-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles20_processes16_run1</v>
       </c>
       <c r="B15">
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D15">
         <v>16</v>
@@ -972,17 +992,21 @@
       <c r="E15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes16_run1 16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f>"parallel-particles"&amp;B16&amp;"-threads"&amp;D16&amp;"-run"&amp;E16</f>
-        <v>parallel-particles20-threads20-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles20_processes20_run1</v>
       </c>
       <c r="B16">
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D16">
         <v>20</v>
@@ -990,17 +1014,21 @@
       <c r="E16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G16" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes20_run1 20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f>"parallel-particles"&amp;B17&amp;"-threads"&amp;D17&amp;"-run"&amp;E17</f>
-        <v>parallel-particles60-threads12-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles60_processes12_run1</v>
       </c>
       <c r="B17">
         <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D17">
         <v>12</v>
@@ -1008,17 +1036,21 @@
       <c r="E17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G17" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes12_run1 12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f>"parallel-particles"&amp;B18&amp;"-threads"&amp;D18&amp;"-run"&amp;E18</f>
-        <v>parallel-particles60-threads24-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles60_processes24_run1</v>
       </c>
       <c r="B18">
         <v>60</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18">
         <v>24</v>
@@ -1026,17 +1058,21 @@
       <c r="E18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G18" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes24_run1 24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f>"parallel-particles"&amp;B19&amp;"-threads"&amp;D19&amp;"-run"&amp;E19</f>
-        <v>parallel-particles60-threads36-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles60_processes36_run1</v>
       </c>
       <c r="B19">
         <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D19">
         <v>36</v>
@@ -1044,17 +1080,21 @@
       <c r="E19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G19" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes36_run1 36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f>"parallel-particles"&amp;B20&amp;"-threads"&amp;D20&amp;"-run"&amp;E20</f>
-        <v>parallel-particles60-threads48-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles60_processes48_run1</v>
       </c>
       <c r="B20">
         <v>60</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20">
         <v>48</v>
@@ -1062,17 +1102,21 @@
       <c r="E20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G20" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes48_run1 48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f>"parallel-particles"&amp;B21&amp;"-threads"&amp;D21&amp;"-run"&amp;E21</f>
-        <v>parallel-particles60-threads60-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles60_processes60_run1</v>
       </c>
       <c r="B21">
         <v>60</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D21">
         <v>60</v>
@@ -1080,17 +1124,21 @@
       <c r="E21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G21" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes60_run1 60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f>"parallel-particles"&amp;B22&amp;"-threads"&amp;D22&amp;"-run"&amp;E22</f>
-        <v>parallel-particles100-threads20-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles100_processes20_run1</v>
       </c>
       <c r="B22">
         <v>100</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D22">
         <v>20</v>
@@ -1098,17 +1146,21 @@
       <c r="E22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G22" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes20_run1 20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f>"parallel-particles"&amp;B23&amp;"-threads"&amp;D23&amp;"-run"&amp;E23</f>
-        <v>parallel-particles100-threads40-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles100_processes40_run1</v>
       </c>
       <c r="B23">
         <v>100</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D23">
         <v>40</v>
@@ -1116,17 +1168,21 @@
       <c r="E23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G23" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes40_run1 40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f>"parallel-particles"&amp;B24&amp;"-threads"&amp;D24&amp;"-run"&amp;E24</f>
-        <v>parallel-particles100-threads60-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles100_processes60_run1</v>
       </c>
       <c r="B24">
         <v>100</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D24">
         <v>60</v>
@@ -1134,17 +1190,21 @@
       <c r="E24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G24" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes60_run1 60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>"parallel-particles"&amp;B25&amp;"-threads"&amp;D25&amp;"-run"&amp;E25</f>
-        <v>parallel-particles100-threads80-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles100_processes80_run1</v>
       </c>
       <c r="B25">
         <v>100</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25">
         <v>80</v>
@@ -1152,17 +1212,21 @@
       <c r="E25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G25" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes80_run1 80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f>"parallel-particles"&amp;B26&amp;"-threads"&amp;D26&amp;"-run"&amp;E26</f>
-        <v>parallel-particles100-threads100-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles100_processes100_run1</v>
       </c>
       <c r="B26">
         <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D26">
         <v>100</v>
@@ -1170,17 +1234,21 @@
       <c r="E26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G26" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes100_run1 100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f>"parallel-particles"&amp;B27&amp;"-threads"&amp;D27&amp;"-run"&amp;E27</f>
-        <v>parallel-particles140-threads28-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles140_processes28_run1</v>
       </c>
       <c r="B27">
         <v>140</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D27">
         <v>28</v>
@@ -1188,17 +1256,21 @@
       <c r="E27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G27" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes28_run1 28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f>"parallel-particles"&amp;B28&amp;"-threads"&amp;D28&amp;"-run"&amp;E28</f>
-        <v>parallel-particles140-threads56-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles140_processes56_run1</v>
       </c>
       <c r="B28">
         <v>140</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D28">
         <v>56</v>
@@ -1206,17 +1278,21 @@
       <c r="E28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G28" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes56_run1 56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f>"parallel-particles"&amp;B29&amp;"-threads"&amp;D29&amp;"-run"&amp;E29</f>
-        <v>parallel-particles140-threads84-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles140_processes84_run1</v>
       </c>
       <c r="B29">
         <v>140</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D29">
         <v>84</v>
@@ -1224,17 +1300,21 @@
       <c r="E29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G29" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes84_run1 84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
-        <f>"parallel-particles"&amp;B30&amp;"-threads"&amp;D30&amp;"-run"&amp;E30</f>
-        <v>parallel-particles140-threads112-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles140_processes112_run1</v>
       </c>
       <c r="B30">
         <v>140</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D30">
         <v>112</v>
@@ -1242,17 +1322,21 @@
       <c r="E30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G30" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes112_run1 112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f>"parallel-particles"&amp;B31&amp;"-threads"&amp;D31&amp;"-run"&amp;E31</f>
-        <v>parallel-particles140-threads140-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles140_processes140_run1</v>
       </c>
       <c r="B31">
         <v>140</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D31">
         <v>140</v>
@@ -1260,17 +1344,21 @@
       <c r="E31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G31" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes140_run1 140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f>"parallel-particles"&amp;B32&amp;"-threads"&amp;D32&amp;"-run"&amp;E32</f>
-        <v>parallel-particles180-threads36-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles180_processes36_run1</v>
       </c>
       <c r="B32">
         <v>180</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D32">
         <v>36</v>
@@ -1278,17 +1366,21 @@
       <c r="E32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G32" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes36_run1 36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f>"parallel-particles"&amp;B33&amp;"-threads"&amp;D33&amp;"-run"&amp;E33</f>
-        <v>parallel-particles180-threads72-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles180_processes72_run1</v>
       </c>
       <c r="B33">
         <v>180</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D33">
         <v>72</v>
@@ -1296,17 +1388,21 @@
       <c r="E33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G33" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes72_run1 72</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f>"parallel-particles"&amp;B34&amp;"-threads"&amp;D34&amp;"-run"&amp;E34</f>
-        <v>parallel-particles180-threads108-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles180_processes108_run1</v>
       </c>
       <c r="B34">
         <v>180</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D34">
         <v>108</v>
@@ -1314,17 +1410,21 @@
       <c r="E34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G34" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes108_run1 108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f>"parallel-particles"&amp;B35&amp;"-threads"&amp;D35&amp;"-run"&amp;E35</f>
-        <v>parallel-particles180-threads144-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles180_processes144_run1</v>
       </c>
       <c r="B35">
         <v>180</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D35">
         <v>144</v>
@@ -1332,17 +1432,21 @@
       <c r="E35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G35" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes144_run1 144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f>"parallel-particles"&amp;B36&amp;"-threads"&amp;D36&amp;"-run"&amp;E36</f>
-        <v>parallel-particles180-threads180-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles180_processes180_run1</v>
       </c>
       <c r="B36">
         <v>180</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D36">
         <v>180</v>
@@ -1350,17 +1454,21 @@
       <c r="E36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G36" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes180_run1 180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f>"parallel-particles"&amp;B37&amp;"-threads"&amp;D37&amp;"-run"&amp;E37</f>
-        <v>parallel-particles220-threads44-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles220_processes44_run1</v>
       </c>
       <c r="B37">
         <v>220</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D37">
         <v>44</v>
@@ -1368,17 +1476,21 @@
       <c r="E37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G37" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes44_run1 44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f>"parallel-particles"&amp;B38&amp;"-threads"&amp;D38&amp;"-run"&amp;E38</f>
-        <v>parallel-particles220-threads88-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles220_processes88_run1</v>
       </c>
       <c r="B38">
         <v>220</v>
       </c>
       <c r="C38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D38">
         <v>88</v>
@@ -1386,17 +1498,21 @@
       <c r="E38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G38" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes88_run1 88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f>"parallel-particles"&amp;B39&amp;"-threads"&amp;D39&amp;"-run"&amp;E39</f>
-        <v>parallel-particles220-threads132-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles220_processes132_run1</v>
       </c>
       <c r="B39">
         <v>220</v>
       </c>
       <c r="C39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D39">
         <v>132</v>
@@ -1404,17 +1520,21 @@
       <c r="E39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G39" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes132_run1 132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f>"parallel-particles"&amp;B40&amp;"-threads"&amp;D40&amp;"-run"&amp;E40</f>
-        <v>parallel-particles220-threads176-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles220_processes176_run1</v>
       </c>
       <c r="B40">
         <v>220</v>
       </c>
       <c r="C40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D40">
         <v>176</v>
@@ -1422,17 +1542,21 @@
       <c r="E40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G40" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes176_run1 176</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f>"parallel-particles"&amp;B41&amp;"-threads"&amp;D41&amp;"-run"&amp;E41</f>
-        <v>parallel-particles220-threads220-run1</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles220_processes220_run1</v>
       </c>
       <c r="B41">
         <v>220</v>
       </c>
       <c r="C41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D41">
         <v>220</v>
@@ -1440,17 +1564,21 @@
       <c r="E41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G41" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes220_run1 220</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f>"parallel-particles"&amp;B42&amp;"-threads"&amp;D42&amp;"-run"&amp;E42</f>
-        <v>parallel-particles20-threads4-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles20_processes4_run2</v>
       </c>
       <c r="B42">
         <v>20</v>
       </c>
       <c r="C42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D42">
         <v>4</v>
@@ -1458,17 +1586,21 @@
       <c r="E42">
         <v>2</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G42" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes4_run2 4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f>"parallel-particles"&amp;B43&amp;"-threads"&amp;D43&amp;"-run"&amp;E43</f>
-        <v>parallel-particles20-threads8-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles20_processes8_run2</v>
       </c>
       <c r="B43">
         <v>20</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D43">
         <v>8</v>
@@ -1476,17 +1608,21 @@
       <c r="E43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G43" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes8_run2 8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f>"parallel-particles"&amp;B44&amp;"-threads"&amp;D44&amp;"-run"&amp;E44</f>
-        <v>parallel-particles20-threads12-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles20_processes12_run2</v>
       </c>
       <c r="B44">
         <v>20</v>
       </c>
       <c r="C44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D44">
         <v>12</v>
@@ -1494,17 +1630,21 @@
       <c r="E44">
         <v>2</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G44" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes12_run2 12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f>"parallel-particles"&amp;B45&amp;"-threads"&amp;D45&amp;"-run"&amp;E45</f>
-        <v>parallel-particles20-threads16-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles20_processes16_run2</v>
       </c>
       <c r="B45">
         <v>20</v>
       </c>
       <c r="C45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D45">
         <v>16</v>
@@ -1512,17 +1652,21 @@
       <c r="E45">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G45" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes16_run2 16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f>"parallel-particles"&amp;B46&amp;"-threads"&amp;D46&amp;"-run"&amp;E46</f>
-        <v>parallel-particles20-threads20-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles20_processes20_run2</v>
       </c>
       <c r="B46">
         <v>20</v>
       </c>
       <c r="C46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D46">
         <v>20</v>
@@ -1530,17 +1674,21 @@
       <c r="E46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G46" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes20_run2 20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f>"parallel-particles"&amp;B47&amp;"-threads"&amp;D47&amp;"-run"&amp;E47</f>
-        <v>parallel-particles60-threads12-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles60_processes12_run2</v>
       </c>
       <c r="B47">
         <v>60</v>
       </c>
       <c r="C47" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D47">
         <v>12</v>
@@ -1548,17 +1696,21 @@
       <c r="E47">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G47" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes12_run2 12</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
-        <f>"parallel-particles"&amp;B48&amp;"-threads"&amp;D48&amp;"-run"&amp;E48</f>
-        <v>parallel-particles60-threads24-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles60_processes24_run2</v>
       </c>
       <c r="B48">
         <v>60</v>
       </c>
       <c r="C48" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D48">
         <v>24</v>
@@ -1566,17 +1718,21 @@
       <c r="E48">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G48" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes24_run2 24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
-        <f>"parallel-particles"&amp;B49&amp;"-threads"&amp;D49&amp;"-run"&amp;E49</f>
-        <v>parallel-particles60-threads36-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles60_processes36_run2</v>
       </c>
       <c r="B49">
         <v>60</v>
       </c>
       <c r="C49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D49">
         <v>36</v>
@@ -1584,17 +1740,21 @@
       <c r="E49">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G49" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes36_run2 36</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
-        <f>"parallel-particles"&amp;B50&amp;"-threads"&amp;D50&amp;"-run"&amp;E50</f>
-        <v>parallel-particles60-threads48-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles60_processes48_run2</v>
       </c>
       <c r="B50">
         <v>60</v>
       </c>
       <c r="C50" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D50">
         <v>48</v>
@@ -1602,17 +1762,21 @@
       <c r="E50">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G50" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes48_run2 48</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
-        <f>"parallel-particles"&amp;B51&amp;"-threads"&amp;D51&amp;"-run"&amp;E51</f>
-        <v>parallel-particles60-threads60-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles60_processes60_run2</v>
       </c>
       <c r="B51">
         <v>60</v>
       </c>
       <c r="C51" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D51">
         <v>60</v>
@@ -1620,17 +1784,21 @@
       <c r="E51">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G51" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes60_run2 60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
-        <f>"parallel-particles"&amp;B52&amp;"-threads"&amp;D52&amp;"-run"&amp;E52</f>
-        <v>parallel-particles100-threads20-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles100_processes20_run2</v>
       </c>
       <c r="B52">
         <v>100</v>
       </c>
       <c r="C52" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D52">
         <v>20</v>
@@ -1638,17 +1806,21 @@
       <c r="E52">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G52" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes20_run2 20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
-        <f>"parallel-particles"&amp;B53&amp;"-threads"&amp;D53&amp;"-run"&amp;E53</f>
-        <v>parallel-particles100-threads40-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles100_processes40_run2</v>
       </c>
       <c r="B53">
         <v>100</v>
       </c>
       <c r="C53" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D53">
         <v>40</v>
@@ -1656,17 +1828,21 @@
       <c r="E53">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G53" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes40_run2 40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
-        <f>"parallel-particles"&amp;B54&amp;"-threads"&amp;D54&amp;"-run"&amp;E54</f>
-        <v>parallel-particles100-threads60-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles100_processes60_run2</v>
       </c>
       <c r="B54">
         <v>100</v>
       </c>
       <c r="C54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D54">
         <v>60</v>
@@ -1674,17 +1850,21 @@
       <c r="E54">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G54" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes60_run2 60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
-        <f>"parallel-particles"&amp;B55&amp;"-threads"&amp;D55&amp;"-run"&amp;E55</f>
-        <v>parallel-particles100-threads80-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles100_processes80_run2</v>
       </c>
       <c r="B55">
         <v>100</v>
       </c>
       <c r="C55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D55">
         <v>80</v>
@@ -1692,17 +1872,21 @@
       <c r="E55">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G55" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes80_run2 80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
-        <f>"parallel-particles"&amp;B56&amp;"-threads"&amp;D56&amp;"-run"&amp;E56</f>
-        <v>parallel-particles100-threads100-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles100_processes100_run2</v>
       </c>
       <c r="B56">
         <v>100</v>
       </c>
       <c r="C56" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D56">
         <v>100</v>
@@ -1710,17 +1894,21 @@
       <c r="E56">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G56" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes100_run2 100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
-        <f>"parallel-particles"&amp;B57&amp;"-threads"&amp;D57&amp;"-run"&amp;E57</f>
-        <v>parallel-particles140-threads28-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles140_processes28_run2</v>
       </c>
       <c r="B57">
         <v>140</v>
       </c>
       <c r="C57" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D57">
         <v>28</v>
@@ -1728,17 +1916,21 @@
       <c r="E57">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G57" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes28_run2 28</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
-        <f>"parallel-particles"&amp;B58&amp;"-threads"&amp;D58&amp;"-run"&amp;E58</f>
-        <v>parallel-particles140-threads56-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles140_processes56_run2</v>
       </c>
       <c r="B58">
         <v>140</v>
       </c>
       <c r="C58" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D58">
         <v>56</v>
@@ -1746,17 +1938,21 @@
       <c r="E58">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G58" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes56_run2 56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
-        <f>"parallel-particles"&amp;B59&amp;"-threads"&amp;D59&amp;"-run"&amp;E59</f>
-        <v>parallel-particles140-threads84-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles140_processes84_run2</v>
       </c>
       <c r="B59">
         <v>140</v>
       </c>
       <c r="C59" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D59">
         <v>84</v>
@@ -1764,17 +1960,21 @@
       <c r="E59">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G59" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes84_run2 84</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
-        <f>"parallel-particles"&amp;B60&amp;"-threads"&amp;D60&amp;"-run"&amp;E60</f>
-        <v>parallel-particles140-threads112-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles140_processes112_run2</v>
       </c>
       <c r="B60">
         <v>140</v>
       </c>
       <c r="C60" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D60">
         <v>112</v>
@@ -1782,17 +1982,21 @@
       <c r="E60">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G60" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes112_run2 112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
-        <f>"parallel-particles"&amp;B61&amp;"-threads"&amp;D61&amp;"-run"&amp;E61</f>
-        <v>parallel-particles140-threads140-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles140_processes140_run2</v>
       </c>
       <c r="B61">
         <v>140</v>
       </c>
       <c r="C61" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D61">
         <v>140</v>
@@ -1800,17 +2004,21 @@
       <c r="E61">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G61" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes140_run2 140</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
-        <f>"parallel-particles"&amp;B62&amp;"-threads"&amp;D62&amp;"-run"&amp;E62</f>
-        <v>parallel-particles180-threads36-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles180_processes36_run2</v>
       </c>
       <c r="B62">
         <v>180</v>
       </c>
       <c r="C62" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D62">
         <v>36</v>
@@ -1818,17 +2026,21 @@
       <c r="E62">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G62" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes36_run2 36</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
-        <f>"parallel-particles"&amp;B63&amp;"-threads"&amp;D63&amp;"-run"&amp;E63</f>
-        <v>parallel-particles180-threads72-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles180_processes72_run2</v>
       </c>
       <c r="B63">
         <v>180</v>
       </c>
       <c r="C63" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D63">
         <v>72</v>
@@ -1836,17 +2048,21 @@
       <c r="E63">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G63" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes72_run2 72</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
-        <f>"parallel-particles"&amp;B64&amp;"-threads"&amp;D64&amp;"-run"&amp;E64</f>
-        <v>parallel-particles180-threads108-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles180_processes108_run2</v>
       </c>
       <c r="B64">
         <v>180</v>
       </c>
       <c r="C64" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D64">
         <v>108</v>
@@ -1854,17 +2070,21 @@
       <c r="E64">
         <v>2</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G64" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes108_run2 108</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="str">
-        <f>"parallel-particles"&amp;B65&amp;"-threads"&amp;D65&amp;"-run"&amp;E65</f>
-        <v>parallel-particles180-threads144-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles180_processes144_run2</v>
       </c>
       <c r="B65">
         <v>180</v>
       </c>
       <c r="C65" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D65">
         <v>144</v>
@@ -1872,17 +2092,21 @@
       <c r="E65">
         <v>2</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G65" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes144_run2 144</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="str">
-        <f>"parallel-particles"&amp;B66&amp;"-threads"&amp;D66&amp;"-run"&amp;E66</f>
-        <v>parallel-particles180-threads180-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles180_processes180_run2</v>
       </c>
       <c r="B66">
         <v>180</v>
       </c>
       <c r="C66" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D66">
         <v>180</v>
@@ -1890,17 +2114,21 @@
       <c r="E66">
         <v>2</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G66" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes180_run2 180</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
-        <f>"parallel-particles"&amp;B67&amp;"-threads"&amp;D67&amp;"-run"&amp;E67</f>
-        <v>parallel-particles220-threads44-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles220_processes44_run2</v>
       </c>
       <c r="B67">
         <v>220</v>
       </c>
       <c r="C67" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D67">
         <v>44</v>
@@ -1908,17 +2136,21 @@
       <c r="E67">
         <v>2</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G67" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes44_run2 44</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="str">
-        <f>"parallel-particles"&amp;B68&amp;"-threads"&amp;D68&amp;"-run"&amp;E68</f>
-        <v>parallel-particles220-threads88-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles220_processes88_run2</v>
       </c>
       <c r="B68">
         <v>220</v>
       </c>
       <c r="C68" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D68">
         <v>88</v>
@@ -1926,17 +2158,21 @@
       <c r="E68">
         <v>2</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G68" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes88_run2 88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="str">
-        <f>"parallel-particles"&amp;B69&amp;"-threads"&amp;D69&amp;"-run"&amp;E69</f>
-        <v>parallel-particles220-threads132-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles220_processes132_run2</v>
       </c>
       <c r="B69">
         <v>220</v>
       </c>
       <c r="C69" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D69">
         <v>132</v>
@@ -1944,17 +2180,21 @@
       <c r="E69">
         <v>2</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G69" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes132_run2 132</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="str">
-        <f>"parallel-particles"&amp;B70&amp;"-threads"&amp;D70&amp;"-run"&amp;E70</f>
-        <v>parallel-particles220-threads176-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles220_processes176_run2</v>
       </c>
       <c r="B70">
         <v>220</v>
       </c>
       <c r="C70" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D70">
         <v>176</v>
@@ -1962,17 +2202,21 @@
       <c r="E70">
         <v>2</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G70" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes176_run2 176</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="str">
-        <f>"parallel-particles"&amp;B71&amp;"-threads"&amp;D71&amp;"-run"&amp;E71</f>
-        <v>parallel-particles220-threads220-run2</v>
+        <f t="shared" si="2"/>
+        <v>parallel_particles220_processes220_run2</v>
       </c>
       <c r="B71">
         <v>220</v>
       </c>
       <c r="C71" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D71">
         <v>220</v>
@@ -1980,9 +2224,23 @@
       <c r="E71">
         <v>2</v>
       </c>
+      <c r="G71" t="str">
+        <f t="shared" si="3"/>
+        <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes220_run2 220</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A11:E11" xr:uid="{F1014102-F14F-4AB9-959E-C9503DEB0969}">
+  <autoFilter ref="A11:E71" xr:uid="{F1014102-F14F-4AB9-959E-C9503DEB0969}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="140"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="4">
+      <filters>
+        <filter val="1"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:E71">
       <sortCondition ref="E11"/>
     </sortState>

</xml_diff>

<commit_message>
refactored directory, run MPI on 12 processes
</commit_message>
<xml_diff>
--- a/run_plan.xlsx
+++ b/run_plan.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukes\Dissertation\Parallel-PSO-OPF-Scalability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE8B067-2502-4938-A2B6-1B4AA056E711}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716B2D57-F412-4B88-8361-02EEEAC73790}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31590" yWindow="705" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="serialRuns" sheetId="1" r:id="rId1"/>
     <sheet name="parallelRuns" sheetId="2" r:id="rId2"/>
+    <sheet name="exta_runs" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">parallelRuns!$A$11:$E$71</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">parallelRuns!$A$22:$G$82</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">serialRuns!$A$1:$D$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="13">
   <si>
     <t>run_name</t>
   </si>
@@ -64,12 +65,27 @@
   <si>
     <t>command</t>
   </si>
+  <si>
+    <t>Particles per process</t>
+  </si>
+  <si>
+    <t>Processes</t>
+  </si>
+  <si>
+    <t>Total Particles</t>
+  </si>
+  <si>
+    <t>particles per process</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +95,29 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -103,18 +142,26 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -697,50 +744,52 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1102CE02-4A00-4625-A7BD-467D2E2DB84D}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:G71"/>
+  <dimension ref="A1:G82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="100.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" customWidth="1"/>
+    <col min="9" max="9" width="4" customWidth="1"/>
+    <col min="10" max="10" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
         <v>0.2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>0.4</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="5">
         <v>0.6</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="5">
         <v>0.8</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="F2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>20</v>
       </c>
       <c r="B3">
@@ -764,8 +813,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>60</v>
       </c>
       <c r="B4">
@@ -789,8 +838,8 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>100</v>
       </c>
       <c r="B5">
@@ -814,8 +863,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>140</v>
       </c>
       <c r="B6">
@@ -839,8 +888,8 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>180</v>
       </c>
       <c r="B7">
@@ -864,8 +913,8 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>220</v>
       </c>
       <c r="B8">
@@ -889,1365 +938,1723 @@
         <v>220</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>12</v>
+      </c>
+      <c r="D11" s="3">
+        <v>24</v>
+      </c>
+      <c r="E11" s="3">
+        <v>48</v>
+      </c>
+      <c r="F11" s="3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <f>B$11*$A12</f>
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <f>C$11*$A12</f>
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <f>D$11*$A12</f>
+        <v>24</v>
+      </c>
+      <c r="E12">
+        <f>E$11*$A12</f>
+        <v>48</v>
+      </c>
+      <c r="F12">
+        <f>F$11*$A12</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <f>B$11*$A13</f>
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <f>C$11*$A13</f>
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <f>D$11*$A13</f>
+        <v>48</v>
+      </c>
+      <c r="E13">
+        <f>E$11*$A13</f>
+        <v>96</v>
+      </c>
+      <c r="F13">
+        <f>F$11*$A13</f>
+        <v>192</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <f>B$11*$A14</f>
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <f>C$11*$A14</f>
+        <v>36</v>
+      </c>
+      <c r="D14">
+        <f>D$11*$A14</f>
+        <v>72</v>
+      </c>
+      <c r="E14">
+        <f>E$11*$A14</f>
+        <v>144</v>
+      </c>
+      <c r="F14">
+        <f>F$11*$A14</f>
+        <v>288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <f>B$11*$A15</f>
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <f>C$11*$A15</f>
+        <v>48</v>
+      </c>
+      <c r="D15">
+        <f>D$11*$A15</f>
+        <v>96</v>
+      </c>
+      <c r="E15">
+        <f>E$11*$A15</f>
+        <v>192</v>
+      </c>
+      <c r="F15">
+        <f>F$11*$A15</f>
+        <v>384</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>5</v>
+      </c>
+      <c r="B16">
+        <f>B$11*$A16</f>
+        <v>5</v>
+      </c>
+      <c r="C16">
+        <f>C$11*$A16</f>
+        <v>60</v>
+      </c>
+      <c r="D16">
+        <f>D$11*$A16</f>
+        <v>120</v>
+      </c>
+      <c r="E16">
+        <f>E$11*$A16</f>
+        <v>240</v>
+      </c>
+      <c r="F16">
+        <f>F$11*$A16</f>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1" t="s">
+      <c r="B22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G22" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="str">
-        <f>"parallel_particles"&amp;B12&amp;"_processes"&amp;D12&amp;"_run"&amp;E12</f>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="str">
+        <f>"parallel_particles"&amp;B23&amp;"_processes"&amp;D23&amp;"_run"&amp;E23</f>
         <v>parallel_particles20_processes4_run1</v>
       </c>
-      <c r="B12">
+      <c r="B23" s="6">
         <v>20</v>
       </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12">
+      <c r="C23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="6">
         <v>4</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="G12" t="str">
-        <f>"srun python parallel_mpi_pso_algorithm.py "&amp;CHAR(34)&amp;CHAR(34) &amp;" 50 "&amp;B12&amp;" 0.25 0.2 0.7 "&amp;A12&amp;" "&amp;D12</f>
+      <c r="E23" s="6">
+        <v>1</v>
+      </c>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6" t="str">
+        <f>"srun python parallel_mpi_pso_algorithm.py "&amp;CHAR(34)&amp;CHAR(34) &amp;" 50 "&amp;B23&amp;" 0.25 0.2 0.7 "&amp;A23&amp;" "&amp;D23</f>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes4_run1 4</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="str">
-        <f t="shared" ref="A13:A71" si="2">"parallel_particles"&amp;B13&amp;"_processes"&amp;D13&amp;"_run"&amp;E13</f>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="str">
+        <f t="shared" ref="A24:A82" si="2">"parallel_particles"&amp;B24&amp;"_processes"&amp;D24&amp;"_run"&amp;E24</f>
         <v>parallel_particles20_processes8_run1</v>
       </c>
-      <c r="B13">
+      <c r="B24" s="6">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13">
+      <c r="C24" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="6">
         <v>8</v>
       </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="G13" t="str">
-        <f t="shared" ref="G13:G71" si="3">"srun python parallel_mpi_pso_algorithm.py "&amp;CHAR(34)&amp;CHAR(34) &amp;" 50 "&amp;B13&amp;" 0.25 0.2 0.7 "&amp;A13&amp;" "&amp;D13</f>
+      <c r="E24" s="6">
+        <v>1</v>
+      </c>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6" t="str">
+        <f t="shared" ref="G24:G82" si="3">"srun python parallel_mpi_pso_algorithm.py "&amp;CHAR(34)&amp;CHAR(34) &amp;" 50 "&amp;B24&amp;" 0.25 0.2 0.7 "&amp;A24&amp;" "&amp;D24</f>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes8_run1 8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="str">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles20_processes12_run1</v>
       </c>
-      <c r="B14">
+      <c r="B25" s="6">
         <v>20</v>
       </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14">
+      <c r="C25" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D25" s="6">
         <v>12</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="G14" t="str">
+      <c r="E25" s="6">
+        <v>1</v>
+      </c>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes12_run1 12</v>
       </c>
     </row>
-    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="str">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles20_processes16_run1</v>
       </c>
-      <c r="B15">
+      <c r="B26" s="6">
         <v>20</v>
       </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15">
+      <c r="C26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="6">
         <v>16</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="G15" t="str">
+      <c r="E26" s="6">
+        <v>1</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes16_run1 16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="str">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles20_processes20_run1</v>
       </c>
-      <c r="B16">
+      <c r="B27" s="6">
         <v>20</v>
       </c>
-      <c r="C16" t="s">
-        <v>5</v>
-      </c>
-      <c r="D16">
+      <c r="C27" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D27" s="6">
         <v>20</v>
       </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="G16" t="str">
+      <c r="E27" s="6">
+        <v>1</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes20_run1 20</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" t="str">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles60_processes12_run1</v>
       </c>
-      <c r="B17">
+      <c r="B28" s="6">
         <v>60</v>
       </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17">
+      <c r="C28" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="6">
         <v>12</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="str">
+      <c r="E28" s="6">
+        <v>1</v>
+      </c>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes12_run1 12</v>
       </c>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="str">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles60_processes24_run1</v>
       </c>
-      <c r="B18">
+      <c r="B29" s="6">
         <v>60</v>
       </c>
-      <c r="C18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18">
+      <c r="C29" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="6">
         <v>24</v>
       </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
-      <c r="G18" t="str">
+      <c r="E29" s="6">
+        <v>1</v>
+      </c>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes24_run1 24</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="str">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles60_processes36_run1</v>
       </c>
-      <c r="B19">
+      <c r="B30" s="6">
         <v>60</v>
       </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19">
+      <c r="C30" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="6">
         <v>36</v>
       </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="G19" t="str">
+      <c r="E30" s="6">
+        <v>1</v>
+      </c>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes36_run1 36</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="str">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles60_processes48_run1</v>
       </c>
-      <c r="B20">
+      <c r="B31" s="6">
         <v>60</v>
       </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-      <c r="D20">
+      <c r="C31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D31" s="6">
         <v>48</v>
       </c>
-      <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="str">
+      <c r="E31" s="6">
+        <v>1</v>
+      </c>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes48_run1 48</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" t="str">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles60_processes60_run1</v>
       </c>
-      <c r="B21">
+      <c r="B32" s="6">
         <v>60</v>
       </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21">
+      <c r="C32" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D32" s="6">
         <v>60</v>
       </c>
-      <c r="E21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="str">
+      <c r="E32" s="6">
+        <v>1</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes60_run1 60</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="str">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles100_processes20_run1</v>
       </c>
-      <c r="B22">
+      <c r="B33" s="6">
         <v>100</v>
       </c>
-      <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22">
+      <c r="C33" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D33" s="6">
         <v>20</v>
       </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="G22" t="str">
+      <c r="E33" s="6">
+        <v>1</v>
+      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes20_run1 20</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="str">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles100_processes40_run1</v>
       </c>
-      <c r="B23">
+      <c r="B34" s="6">
         <v>100</v>
       </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-      <c r="D23">
+      <c r="C34" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D34" s="6">
         <v>40</v>
       </c>
-      <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="G23" t="str">
+      <c r="E34" s="6">
+        <v>1</v>
+      </c>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes40_run1 40</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" t="str">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles100_processes60_run1</v>
       </c>
-      <c r="B24">
+      <c r="B35" s="6">
         <v>100</v>
       </c>
-      <c r="C24" t="s">
-        <v>5</v>
-      </c>
-      <c r="D24">
+      <c r="C35" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="6">
         <v>60</v>
       </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="G24" t="str">
+      <c r="E35" s="6">
+        <v>1</v>
+      </c>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes60_run1 60</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" t="str">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles100_processes80_run1</v>
       </c>
-      <c r="B25">
+      <c r="B36" s="6">
         <v>100</v>
       </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25">
+      <c r="C36" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="6">
         <v>80</v>
       </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="G25" t="str">
+      <c r="E36" s="6">
+        <v>1</v>
+      </c>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes80_run1 80</v>
       </c>
     </row>
-    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" t="str">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles100_processes100_run1</v>
       </c>
-      <c r="B26">
+      <c r="B37" s="6">
         <v>100</v>
       </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26">
+      <c r="C37" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D37" s="6">
         <v>100</v>
       </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="G26" t="str">
+      <c r="E37" s="6">
+        <v>1</v>
+      </c>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes100_run1 100</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" t="str">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles140_processes28_run1</v>
       </c>
-      <c r="B27">
+      <c r="B38" s="6">
         <v>140</v>
       </c>
-      <c r="C27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27">
+      <c r="C38" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D38" s="6">
         <v>28</v>
       </c>
-      <c r="E27">
-        <v>1</v>
-      </c>
-      <c r="G27" t="str">
+      <c r="E38" s="6">
+        <v>1</v>
+      </c>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes28_run1 28</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" t="str">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles140_processes56_run1</v>
       </c>
-      <c r="B28">
+      <c r="B39" s="6">
         <v>140</v>
       </c>
-      <c r="C28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28">
+      <c r="C39" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="6">
         <v>56</v>
       </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="G28" t="str">
+      <c r="E39" s="6">
+        <v>1</v>
+      </c>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes56_run1 56</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="str">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles140_processes84_run1</v>
       </c>
-      <c r="B29">
+      <c r="B40" s="6">
         <v>140</v>
       </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29">
+      <c r="C40" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D40" s="6">
         <v>84</v>
       </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="G29" t="str">
+      <c r="E40" s="6">
+        <v>1</v>
+      </c>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes84_run1 84</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" t="str">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles140_processes112_run1</v>
       </c>
-      <c r="B30">
+      <c r="B41" s="6">
         <v>140</v>
       </c>
-      <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30">
+      <c r="C41" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="6">
         <v>112</v>
       </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="G30" t="str">
+      <c r="E41" s="6">
+        <v>1</v>
+      </c>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes112_run1 112</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="str">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles140_processes140_run1</v>
       </c>
-      <c r="B31">
+      <c r="B42" s="6">
         <v>140</v>
       </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31">
+      <c r="C42" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="6">
         <v>140</v>
       </c>
-      <c r="E31">
-        <v>1</v>
-      </c>
-      <c r="G31" t="str">
+      <c r="E42" s="6">
+        <v>1</v>
+      </c>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes140_run1 140</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="str">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles180_processes36_run1</v>
       </c>
-      <c r="B32">
+      <c r="B43" s="6">
         <v>180</v>
       </c>
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32">
+      <c r="C43" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="6">
         <v>36</v>
       </c>
-      <c r="E32">
-        <v>1</v>
-      </c>
-      <c r="G32" t="str">
+      <c r="E43" s="6">
+        <v>1</v>
+      </c>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes36_run1 36</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="str">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles180_processes72_run1</v>
       </c>
-      <c r="B33">
+      <c r="B44" s="6">
         <v>180</v>
       </c>
-      <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33">
+      <c r="C44" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="6">
         <v>72</v>
       </c>
-      <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="G33" t="str">
+      <c r="E44" s="6">
+        <v>1</v>
+      </c>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes72_run1 72</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" t="str">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles180_processes108_run1</v>
       </c>
-      <c r="B34">
+      <c r="B45" s="6">
         <v>180</v>
       </c>
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34">
+      <c r="C45" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="6">
         <v>108</v>
       </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="G34" t="str">
+      <c r="E45" s="6">
+        <v>1</v>
+      </c>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes108_run1 108</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" t="str">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles180_processes144_run1</v>
       </c>
-      <c r="B35">
+      <c r="B46" s="6">
         <v>180</v>
       </c>
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35">
+      <c r="C46" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="6">
         <v>144</v>
       </c>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="G35" t="str">
+      <c r="E46" s="6">
+        <v>1</v>
+      </c>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes144_run1 144</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" t="str">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles180_processes180_run1</v>
       </c>
-      <c r="B36">
+      <c r="B47" s="6">
         <v>180</v>
       </c>
-      <c r="C36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36">
+      <c r="C47" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="6">
         <v>180</v>
       </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="G36" t="str">
+      <c r="E47" s="6">
+        <v>1</v>
+      </c>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes180_run1 180</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="str">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles220_processes44_run1</v>
       </c>
-      <c r="B37">
+      <c r="B48" s="6">
         <v>220</v>
       </c>
-      <c r="C37" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37">
+      <c r="C48" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="6">
         <v>44</v>
       </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="G37" t="str">
+      <c r="E48" s="6">
+        <v>1</v>
+      </c>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes44_run1 44</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="str">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles220_processes88_run1</v>
       </c>
-      <c r="B38">
+      <c r="B49" s="6">
         <v>220</v>
       </c>
-      <c r="C38" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38">
+      <c r="C49" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D49" s="6">
         <v>88</v>
       </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="G38" t="str">
+      <c r="E49" s="6">
+        <v>1</v>
+      </c>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes88_run1 88</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="str">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles220_processes132_run1</v>
       </c>
-      <c r="B39">
+      <c r="B50" s="6">
         <v>220</v>
       </c>
-      <c r="C39" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39">
+      <c r="C50" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D50" s="6">
         <v>132</v>
       </c>
-      <c r="E39">
-        <v>1</v>
-      </c>
-      <c r="G39" t="str">
+      <c r="E50" s="6">
+        <v>1</v>
+      </c>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes132_run1 132</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" t="str">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles220_processes176_run1</v>
       </c>
-      <c r="B40">
+      <c r="B51" s="6">
         <v>220</v>
       </c>
-      <c r="C40" t="s">
-        <v>5</v>
-      </c>
-      <c r="D40">
+      <c r="C51" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="6">
         <v>176</v>
       </c>
-      <c r="E40">
-        <v>1</v>
-      </c>
-      <c r="G40" t="str">
+      <c r="E51" s="6">
+        <v>1</v>
+      </c>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes176_run1 176</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" t="str">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles220_processes220_run1</v>
       </c>
-      <c r="B41">
+      <c r="B52" s="6">
         <v>220</v>
       </c>
-      <c r="C41" t="s">
-        <v>5</v>
-      </c>
-      <c r="D41">
+      <c r="C52" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D52" s="6">
         <v>220</v>
       </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="G41" t="str">
+      <c r="E52" s="6">
+        <v>1</v>
+      </c>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes220_run1 220</v>
       </c>
     </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" t="str">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles20_processes4_run2</v>
       </c>
-      <c r="B42">
+      <c r="B53" s="6">
         <v>20</v>
       </c>
-      <c r="C42" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42">
+      <c r="C53" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="6">
         <v>4</v>
       </c>
-      <c r="E42">
-        <v>2</v>
-      </c>
-      <c r="G42" t="str">
+      <c r="E53" s="6">
+        <v>2</v>
+      </c>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes4_run2 4</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" t="str">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles20_processes8_run2</v>
       </c>
-      <c r="B43">
+      <c r="B54" s="6">
         <v>20</v>
       </c>
-      <c r="C43" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43">
+      <c r="C54" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D54" s="6">
         <v>8</v>
       </c>
-      <c r="E43">
-        <v>2</v>
-      </c>
-      <c r="G43" t="str">
+      <c r="E54" s="6">
+        <v>2</v>
+      </c>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes8_run2 8</v>
       </c>
     </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" t="str">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles20_processes12_run2</v>
       </c>
-      <c r="B44">
+      <c r="B55" s="6">
         <v>20</v>
       </c>
-      <c r="C44" t="s">
-        <v>5</v>
-      </c>
-      <c r="D44">
+      <c r="C55" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="6">
         <v>12</v>
       </c>
-      <c r="E44">
-        <v>2</v>
-      </c>
-      <c r="G44" t="str">
+      <c r="E55" s="6">
+        <v>2</v>
+      </c>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes12_run2 12</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" t="str">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles20_processes16_run2</v>
       </c>
-      <c r="B45">
+      <c r="B56" s="6">
         <v>20</v>
       </c>
-      <c r="C45" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45">
+      <c r="C56" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D56" s="6">
         <v>16</v>
       </c>
-      <c r="E45">
-        <v>2</v>
-      </c>
-      <c r="G45" t="str">
+      <c r="E56" s="6">
+        <v>2</v>
+      </c>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes16_run2 16</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A46" t="str">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles20_processes20_run2</v>
       </c>
-      <c r="B46">
+      <c r="B57" s="6">
         <v>20</v>
       </c>
-      <c r="C46" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46">
+      <c r="C57" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="6">
         <v>20</v>
       </c>
-      <c r="E46">
-        <v>2</v>
-      </c>
-      <c r="G46" t="str">
+      <c r="E57" s="6">
+        <v>2</v>
+      </c>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 20 0.25 0.2 0.7 parallel_particles20_processes20_run2 20</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A47" t="str">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles60_processes12_run2</v>
       </c>
-      <c r="B47">
+      <c r="B58" s="6">
         <v>60</v>
       </c>
-      <c r="C47" t="s">
-        <v>5</v>
-      </c>
-      <c r="D47">
+      <c r="C58" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D58" s="6">
         <v>12</v>
       </c>
-      <c r="E47">
-        <v>2</v>
-      </c>
-      <c r="G47" t="str">
+      <c r="E58" s="6">
+        <v>2</v>
+      </c>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes12_run2 12</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A48" t="str">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles60_processes24_run2</v>
       </c>
-      <c r="B48">
+      <c r="B59" s="6">
         <v>60</v>
       </c>
-      <c r="C48" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48">
+      <c r="C59" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="6">
         <v>24</v>
       </c>
-      <c r="E48">
-        <v>2</v>
-      </c>
-      <c r="G48" t="str">
+      <c r="E59" s="6">
+        <v>2</v>
+      </c>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes24_run2 24</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" t="str">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles60_processes36_run2</v>
       </c>
-      <c r="B49">
+      <c r="B60" s="6">
         <v>60</v>
       </c>
-      <c r="C49" t="s">
-        <v>5</v>
-      </c>
-      <c r="D49">
+      <c r="C60" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D60" s="6">
         <v>36</v>
       </c>
-      <c r="E49">
-        <v>2</v>
-      </c>
-      <c r="G49" t="str">
+      <c r="E60" s="6">
+        <v>2</v>
+      </c>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes36_run2 36</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A50" t="str">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles60_processes48_run2</v>
       </c>
-      <c r="B50">
+      <c r="B61" s="6">
         <v>60</v>
       </c>
-      <c r="C50" t="s">
-        <v>5</v>
-      </c>
-      <c r="D50">
+      <c r="C61" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D61" s="6">
         <v>48</v>
       </c>
-      <c r="E50">
-        <v>2</v>
-      </c>
-      <c r="G50" t="str">
+      <c r="E61" s="6">
+        <v>2</v>
+      </c>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes48_run2 48</v>
       </c>
     </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" t="str">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles60_processes60_run2</v>
       </c>
-      <c r="B51">
+      <c r="B62" s="6">
         <v>60</v>
       </c>
-      <c r="C51" t="s">
-        <v>5</v>
-      </c>
-      <c r="D51">
+      <c r="C62" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62" s="6">
         <v>60</v>
       </c>
-      <c r="E51">
-        <v>2</v>
-      </c>
-      <c r="G51" t="str">
+      <c r="E62" s="6">
+        <v>2</v>
+      </c>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 60 0.25 0.2 0.7 parallel_particles60_processes60_run2 60</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A52" t="str">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles100_processes20_run2</v>
       </c>
-      <c r="B52">
+      <c r="B63" s="6">
         <v>100</v>
       </c>
-      <c r="C52" t="s">
-        <v>5</v>
-      </c>
-      <c r="D52">
+      <c r="C63" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="6">
         <v>20</v>
       </c>
-      <c r="E52">
-        <v>2</v>
-      </c>
-      <c r="G52" t="str">
+      <c r="E63" s="6">
+        <v>2</v>
+      </c>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes20_run2 20</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A53" t="str">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles100_processes40_run2</v>
       </c>
-      <c r="B53">
+      <c r="B64" s="6">
         <v>100</v>
       </c>
-      <c r="C53" t="s">
-        <v>5</v>
-      </c>
-      <c r="D53">
+      <c r="C64" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D64" s="6">
         <v>40</v>
       </c>
-      <c r="E53">
-        <v>2</v>
-      </c>
-      <c r="G53" t="str">
+      <c r="E64" s="6">
+        <v>2</v>
+      </c>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes40_run2 40</v>
       </c>
     </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" t="str">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles100_processes60_run2</v>
       </c>
-      <c r="B54">
+      <c r="B65" s="6">
         <v>100</v>
       </c>
-      <c r="C54" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54">
+      <c r="C65" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="6">
         <v>60</v>
       </c>
-      <c r="E54">
-        <v>2</v>
-      </c>
-      <c r="G54" t="str">
+      <c r="E65" s="6">
+        <v>2</v>
+      </c>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes60_run2 60</v>
       </c>
     </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A55" t="str">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles100_processes80_run2</v>
       </c>
-      <c r="B55">
+      <c r="B66" s="6">
         <v>100</v>
       </c>
-      <c r="C55" t="s">
-        <v>5</v>
-      </c>
-      <c r="D55">
+      <c r="C66" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D66" s="6">
         <v>80</v>
       </c>
-      <c r="E55">
-        <v>2</v>
-      </c>
-      <c r="G55" t="str">
+      <c r="E66" s="6">
+        <v>2</v>
+      </c>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes80_run2 80</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A56" t="str">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles100_processes100_run2</v>
       </c>
-      <c r="B56">
+      <c r="B67" s="6">
         <v>100</v>
       </c>
-      <c r="C56" t="s">
-        <v>5</v>
-      </c>
-      <c r="D56">
+      <c r="C67" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="6">
         <v>100</v>
       </c>
-      <c r="E56">
-        <v>2</v>
-      </c>
-      <c r="G56" t="str">
+      <c r="E67" s="6">
+        <v>2</v>
+      </c>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 100 0.25 0.2 0.7 parallel_particles100_processes100_run2 100</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57" t="str">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles140_processes28_run2</v>
       </c>
-      <c r="B57">
+      <c r="B68" s="6">
         <v>140</v>
       </c>
-      <c r="C57" t="s">
-        <v>5</v>
-      </c>
-      <c r="D57">
+      <c r="C68" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D68" s="6">
         <v>28</v>
       </c>
-      <c r="E57">
-        <v>2</v>
-      </c>
-      <c r="G57" t="str">
+      <c r="E68" s="6">
+        <v>2</v>
+      </c>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes28_run2 28</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A58" t="str">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles140_processes56_run2</v>
       </c>
-      <c r="B58">
+      <c r="B69" s="6">
         <v>140</v>
       </c>
-      <c r="C58" t="s">
-        <v>5</v>
-      </c>
-      <c r="D58">
+      <c r="C69" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="6">
         <v>56</v>
       </c>
-      <c r="E58">
-        <v>2</v>
-      </c>
-      <c r="G58" t="str">
+      <c r="E69" s="6">
+        <v>2</v>
+      </c>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes56_run2 56</v>
       </c>
     </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A59" t="str">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles140_processes84_run2</v>
       </c>
-      <c r="B59">
+      <c r="B70" s="6">
         <v>140</v>
       </c>
-      <c r="C59" t="s">
-        <v>5</v>
-      </c>
-      <c r="D59">
+      <c r="C70" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="6">
         <v>84</v>
       </c>
-      <c r="E59">
-        <v>2</v>
-      </c>
-      <c r="G59" t="str">
+      <c r="E70" s="6">
+        <v>2</v>
+      </c>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes84_run2 84</v>
       </c>
     </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60" t="str">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles140_processes112_run2</v>
       </c>
-      <c r="B60">
+      <c r="B71" s="6">
         <v>140</v>
       </c>
-      <c r="C60" t="s">
-        <v>5</v>
-      </c>
-      <c r="D60">
+      <c r="C71" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D71" s="6">
         <v>112</v>
       </c>
-      <c r="E60">
-        <v>2</v>
-      </c>
-      <c r="G60" t="str">
+      <c r="E71" s="6">
+        <v>2</v>
+      </c>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes112_run2 112</v>
       </c>
     </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A61" t="str">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles140_processes140_run2</v>
       </c>
-      <c r="B61">
+      <c r="B72" s="6">
         <v>140</v>
       </c>
-      <c r="C61" t="s">
-        <v>5</v>
-      </c>
-      <c r="D61">
+      <c r="C72" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="6">
         <v>140</v>
       </c>
-      <c r="E61">
-        <v>2</v>
-      </c>
-      <c r="G61" t="str">
+      <c r="E72" s="6">
+        <v>2</v>
+      </c>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 140 0.25 0.2 0.7 parallel_particles140_processes140_run2 140</v>
       </c>
     </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A62" t="str">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles180_processes36_run2</v>
       </c>
-      <c r="B62">
+      <c r="B73" s="6">
         <v>180</v>
       </c>
-      <c r="C62" t="s">
-        <v>5</v>
-      </c>
-      <c r="D62">
+      <c r="C73" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73" s="6">
         <v>36</v>
       </c>
-      <c r="E62">
-        <v>2</v>
-      </c>
-      <c r="G62" t="str">
+      <c r="E73" s="6">
+        <v>2</v>
+      </c>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes36_run2 36</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A63" t="str">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles180_processes72_run2</v>
       </c>
-      <c r="B63">
+      <c r="B74" s="6">
         <v>180</v>
       </c>
-      <c r="C63" t="s">
-        <v>5</v>
-      </c>
-      <c r="D63">
+      <c r="C74" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74" s="6">
         <v>72</v>
       </c>
-      <c r="E63">
-        <v>2</v>
-      </c>
-      <c r="G63" t="str">
+      <c r="E74" s="6">
+        <v>2</v>
+      </c>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes72_run2 72</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A64" t="str">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles180_processes108_run2</v>
       </c>
-      <c r="B64">
+      <c r="B75" s="6">
         <v>180</v>
       </c>
-      <c r="C64" t="s">
-        <v>5</v>
-      </c>
-      <c r="D64">
+      <c r="C75" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D75" s="6">
         <v>108</v>
       </c>
-      <c r="E64">
-        <v>2</v>
-      </c>
-      <c r="G64" t="str">
+      <c r="E75" s="6">
+        <v>2</v>
+      </c>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes108_run2 108</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A65" t="str">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles180_processes144_run2</v>
       </c>
-      <c r="B65">
+      <c r="B76" s="6">
         <v>180</v>
       </c>
-      <c r="C65" t="s">
-        <v>5</v>
-      </c>
-      <c r="D65">
+      <c r="C76" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D76" s="6">
         <v>144</v>
       </c>
-      <c r="E65">
-        <v>2</v>
-      </c>
-      <c r="G65" t="str">
+      <c r="E76" s="6">
+        <v>2</v>
+      </c>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes144_run2 144</v>
       </c>
     </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A66" t="str">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles180_processes180_run2</v>
       </c>
-      <c r="B66">
+      <c r="B77" s="6">
         <v>180</v>
       </c>
-      <c r="C66" t="s">
-        <v>5</v>
-      </c>
-      <c r="D66">
+      <c r="C77" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D77" s="6">
         <v>180</v>
       </c>
-      <c r="E66">
-        <v>2</v>
-      </c>
-      <c r="G66" t="str">
+      <c r="E77" s="6">
+        <v>2</v>
+      </c>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 180 0.25 0.2 0.7 parallel_particles180_processes180_run2 180</v>
       </c>
     </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A67" t="str">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles220_processes44_run2</v>
       </c>
-      <c r="B67">
+      <c r="B78" s="6">
         <v>220</v>
       </c>
-      <c r="C67" t="s">
-        <v>5</v>
-      </c>
-      <c r="D67">
+      <c r="C78" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D78" s="6">
         <v>44</v>
       </c>
-      <c r="E67">
-        <v>2</v>
-      </c>
-      <c r="G67" t="str">
+      <c r="E78" s="6">
+        <v>2</v>
+      </c>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes44_run2 44</v>
       </c>
     </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A68" t="str">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles220_processes88_run2</v>
       </c>
-      <c r="B68">
+      <c r="B79" s="6">
         <v>220</v>
       </c>
-      <c r="C68" t="s">
-        <v>5</v>
-      </c>
-      <c r="D68">
+      <c r="C79" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" s="6">
         <v>88</v>
       </c>
-      <c r="E68">
-        <v>2</v>
-      </c>
-      <c r="G68" t="str">
+      <c r="E79" s="6">
+        <v>2</v>
+      </c>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes88_run2 88</v>
       </c>
     </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A69" t="str">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles220_processes132_run2</v>
       </c>
-      <c r="B69">
+      <c r="B80" s="6">
         <v>220</v>
       </c>
-      <c r="C69" t="s">
-        <v>5</v>
-      </c>
-      <c r="D69">
+      <c r="C80" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" s="6">
         <v>132</v>
       </c>
-      <c r="E69">
-        <v>2</v>
-      </c>
-      <c r="G69" t="str">
+      <c r="E80" s="6">
+        <v>2</v>
+      </c>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes132_run2 132</v>
       </c>
     </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A70" t="str">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles220_processes176_run2</v>
       </c>
-      <c r="B70">
+      <c r="B81" s="6">
         <v>220</v>
       </c>
-      <c r="C70" t="s">
-        <v>5</v>
-      </c>
-      <c r="D70">
+      <c r="C81" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" s="6">
         <v>176</v>
       </c>
-      <c r="E70">
-        <v>2</v>
-      </c>
-      <c r="G70" t="str">
+      <c r="E81" s="6">
+        <v>2</v>
+      </c>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes176_run2 176</v>
       </c>
     </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A71" t="str">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="6" t="str">
         <f t="shared" si="2"/>
         <v>parallel_particles220_processes220_run2</v>
       </c>
-      <c r="B71">
+      <c r="B82" s="6">
         <v>220</v>
       </c>
-      <c r="C71" t="s">
-        <v>5</v>
-      </c>
-      <c r="D71">
+      <c r="C82" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D82" s="6">
         <v>220</v>
       </c>
-      <c r="E71">
-        <v>2</v>
-      </c>
-      <c r="G71" t="str">
+      <c r="E82" s="6">
+        <v>2</v>
+      </c>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6" t="str">
         <f t="shared" si="3"/>
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 220 0.25 0.2 0.7 parallel_particles220_processes220_run2 220</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A11:E71" xr:uid="{F1014102-F14F-4AB9-959E-C9503DEB0969}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="140"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="4">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A12:E71">
-      <sortCondition ref="E11"/>
-    </sortState>
-  </autoFilter>
-  <mergeCells count="1">
+  <autoFilter ref="A22:G82" xr:uid="{9457D072-137A-4B67-857F-02B4C3EAD8AB}"/>
+  <mergeCells count="2">
     <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B10:F10"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{987A5B21-304A-4397-8272-6ECB4F7F36B8}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>60</v>
+      </c>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <f>A2*B2</f>
+        <v>720</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <f>A3*B3</f>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <v>36</v>
+      </c>
+      <c r="C4">
+        <f>A4*B4</f>
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>60</v>
+      </c>
+      <c r="B5">
+        <v>48</v>
+      </c>
+      <c r="C5">
+        <f>A5*B5</f>
+        <v>2880</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <v>60</v>
+      </c>
+      <c r="C6">
+        <f>A6*B6</f>
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <f>A7*B7</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <f>A8*B8</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <f>A9*B9</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <f>A10*B10</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <f>A11*B11</f>
+        <v>400</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
sychronized with online repo
</commit_message>
<xml_diff>
--- a/run_plan.xlsx
+++ b/run_plan.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukes\Dissertation\Parallel-PSO-OPF-Scalability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B65B23-524F-44E4-B43E-A502A68E420C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4504BE26-F8D2-4466-915D-17B73B9152C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32550" yWindow="2055" windowWidth="21600" windowHeight="11835" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="serialRuns" sheetId="1" r:id="rId1"/>
     <sheet name="parallelRuns" sheetId="2" r:id="rId2"/>
     <sheet name="extra_runs" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">parallelRuns!$A$22:$G$82</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">serialRuns!$A$1:$D$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="16">
   <si>
     <t>run_name</t>
   </si>
@@ -81,12 +81,21 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>particles</t>
+  </si>
+  <si>
+    <t>processes</t>
+  </si>
+  <si>
+    <t>min_runtime</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +147,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FF262730"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FFFF0000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -152,12 +173,64 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -166,7 +239,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -185,6 +258,30 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -775,8 +872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1102CE02-4A00-4625-A7BD-467D2E2DB84D}">
   <dimension ref="A1:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3020,4 +3117,149 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A4D4AE-7436-45D6-BD3C-D4B5923ED9C3}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="13">
+        <v>48</v>
+      </c>
+      <c r="B2" s="14">
+        <v>1</v>
+      </c>
+      <c r="C2" s="15">
+        <v>178.20760000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="13">
+        <v>48</v>
+      </c>
+      <c r="B3" s="14">
+        <v>12</v>
+      </c>
+      <c r="C3" s="15">
+        <v>20.2334</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="13">
+        <v>48</v>
+      </c>
+      <c r="B4" s="14">
+        <v>24</v>
+      </c>
+      <c r="C4" s="15">
+        <v>13.4581</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="13">
+        <v>48</v>
+      </c>
+      <c r="B5" s="14">
+        <v>48</v>
+      </c>
+      <c r="C5" s="15">
+        <v>10.029</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="13">
+        <v>96</v>
+      </c>
+      <c r="B6" s="14">
+        <v>1</v>
+      </c>
+      <c r="C6" s="15">
+        <v>355.4391</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13">
+        <v>96</v>
+      </c>
+      <c r="B7" s="14">
+        <v>24</v>
+      </c>
+      <c r="C7" s="15">
+        <v>20.783899999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13">
+        <v>96</v>
+      </c>
+      <c r="B8" s="14">
+        <v>48</v>
+      </c>
+      <c r="C8" s="15">
+        <v>13.7822</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="13">
+        <v>96</v>
+      </c>
+      <c r="B9" s="14">
+        <v>96</v>
+      </c>
+      <c r="C9" s="15">
+        <v>10.606</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="16"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="18"/>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="13"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="15"/>
+    </row>
+    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="13"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="15"/>
+    </row>
+    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="15"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="15"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added network viewer, analysed 30 bus run data
</commit_message>
<xml_diff>
--- a/run_plan.xlsx
+++ b/run_plan.xlsx
@@ -1,47 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mukes\Dissertation\Parallel-PSO-OPF-Scalability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4504BE26-F8D2-4466-915D-17B73B9152C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE79250-449A-4949-A7CC-131DF0EBA0BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32550" yWindow="2055" windowWidth="21600" windowHeight="11835" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1812" yWindow="576" windowWidth="20892" windowHeight="11592" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="serialRuns" sheetId="1" r:id="rId1"/>
     <sheet name="parallelRuns" sheetId="2" r:id="rId2"/>
     <sheet name="extra_runs" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
+    <sheet name="doubling-particles" sheetId="4" r:id="rId4"/>
+    <sheet name="fitness" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">parallelRuns!$A$22:$G$82</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">serialRuns!$A$1:$D$19</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="24">
   <si>
     <t>run_name</t>
   </si>
@@ -90,12 +82,40 @@
   <si>
     <t>min_runtime</t>
   </si>
+  <si>
+    <t>nparticles</t>
+  </si>
+  <si>
+    <t>avg_p_loss_14_bus</t>
+  </si>
+  <si>
+    <t>avg_p_loss_30_bus</t>
+  </si>
+  <si>
+    <t>run1</t>
+  </si>
+  <si>
+    <t>run2</t>
+  </si>
+  <si>
+    <t>run3</t>
+  </si>
+  <si>
+    <t>run4</t>
+  </si>
+  <si>
+    <t>run5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="170" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +179,18 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF262730"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="13.5"/>
+      <color rgb="FF1E6777"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -173,7 +205,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -233,13 +265,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFD5DAE5"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFD5DAE5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -256,9 +299,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -283,6 +323,26 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
@@ -300,6 +360,1135 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Power</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> Loss vs Number of Particles</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>14-bus-system</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>fitness!$A$2:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>288</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>384</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>fitness!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1.6308</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2867799999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95776000000000006</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.87073999999999996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.75473999999999997</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.71301999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.64498000000000011</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-261E-4AA1-85DA-922254E9E48A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>30-bus-system</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>fitness!$B$11:$B$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>3.2825200000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.2276600000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.4554</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1260000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8787200000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8597600000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7406399999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-261E-4AA1-85DA-922254E9E48A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2053084447"/>
+        <c:axId val="2053084863"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2053084447"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Number of Particles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2053084863"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2053084863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Power Loss (MW)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2053084447"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>270510</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>129540</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43765672-1A3E-4686-9C85-58D62D591B4F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -571,14 +1760,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -592,7 +1781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f t="shared" ref="A2:A19" si="0">"serial-particles"&amp;B2&amp;"-run"&amp;D2</f>
         <v>serial-particles20-run1</v>
@@ -607,7 +1796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
         <v>serial-particles20-run2</v>
@@ -622,7 +1811,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
         <v>serial-particles20-run3</v>
@@ -637,7 +1826,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
         <v>serial-particles60-run1</v>
@@ -652,7 +1841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
         <v>serial-particles60-run2</v>
@@ -667,7 +1856,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
         <v>serial-particles60-run3</v>
@@ -682,7 +1871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
         <v>serial-particles100-run1</v>
@@ -697,7 +1886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
         <v>serial-particles100-run2</v>
@@ -712,7 +1901,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
         <v>serial-particles100-run3</v>
@@ -727,7 +1916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
         <v>serial-particles140-run1</v>
@@ -742,7 +1931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
         <v>serial-particles140-run2</v>
@@ -757,7 +1946,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
         <v>serial-particles140-run3</v>
@@ -772,7 +1961,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
         <v>serial-particles180-run1</v>
@@ -787,7 +1976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
         <v>serial-particles180-run2</v>
@@ -802,7 +1991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
         <v>serial-particles180-run3</v>
@@ -817,7 +2006,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
         <v>serial-particles220-run1</v>
@@ -832,7 +2021,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
         <v>serial-particles220-run2</v>
@@ -847,7 +2036,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
         <v>serial-particles220-run3</v>
@@ -873,31 +2062,31 @@
   <dimension ref="A1:G97"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:F16"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
-    <col min="7" max="7" width="100.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.88671875" customWidth="1"/>
+    <col min="7" max="7" width="100.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" customWidth="1"/>
     <col min="9" max="9" width="4" customWidth="1"/>
-    <col min="10" max="10" width="6.7109375" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -917,7 +2106,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>20</v>
       </c>
@@ -942,7 +2131,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>60</v>
       </c>
@@ -967,7 +2156,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>100</v>
       </c>
@@ -992,7 +2181,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>140</v>
       </c>
@@ -1017,7 +2206,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>180</v>
       </c>
@@ -1042,7 +2231,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>220</v>
       </c>
@@ -1067,16 +2256,16 @@
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1096,7 +2285,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>1</v>
       </c>
@@ -1121,7 +2310,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>2</v>
       </c>
@@ -1146,7 +2335,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>3</v>
       </c>
@@ -1171,7 +2360,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>4</v>
       </c>
@@ -1196,7 +2385,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>5</v>
       </c>
@@ -1221,12 +2410,12 @@
         <v>480</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>0</v>
       </c>
@@ -1247,7 +2436,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="8" t="str">
         <f>"parallel_particles"&amp;B23*D23&amp;"_processes"&amp;D23&amp;"_run"&amp;E23</f>
         <v>parallel_particles12_processes12_run1</v>
@@ -1270,7 +2459,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 1 0.25 0.2 0.7 parallel_particles12_processes12_run1 12</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="8" t="str">
         <f t="shared" ref="A24:A87" si="3">"parallel_particles"&amp;B24*D24&amp;"_processes"&amp;D24&amp;"_run"&amp;E24</f>
         <v>parallel_particles24_processes12_run1</v>
@@ -1293,7 +2482,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 2 0.25 0.2 0.7 parallel_particles24_processes12_run1 12</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles36_processes12_run1</v>
@@ -1316,7 +2505,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 3 0.25 0.2 0.7 parallel_particles36_processes12_run1 12</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles48_processes12_run1</v>
@@ -1339,7 +2528,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 4 0.25 0.2 0.7 parallel_particles48_processes12_run1 12</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles60_processes12_run1</v>
@@ -1362,7 +2551,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 5 0.25 0.2 0.7 parallel_particles60_processes12_run1 12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles1_processes1_run1</v>
@@ -1385,7 +2574,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 1 0.25 0.2 0.7 parallel_particles1_processes1_run1 1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles2_processes1_run1</v>
@@ -1408,7 +2597,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 2 0.25 0.2 0.7 parallel_particles2_processes1_run1 1</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles3_processes1_run1</v>
@@ -1431,7 +2620,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 3 0.25 0.2 0.7 parallel_particles3_processes1_run1 1</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles4_processes1_run1</v>
@@ -1454,7 +2643,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 4 0.25 0.2 0.7 parallel_particles4_processes1_run1 1</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles5_processes1_run1</v>
@@ -1477,7 +2666,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 5 0.25 0.2 0.7 parallel_particles5_processes1_run1 1</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles24_processes24_run1</v>
@@ -1500,7 +2689,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 1 0.25 0.2 0.7 parallel_particles24_processes24_run1 24</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles48_processes24_run1</v>
@@ -1523,7 +2712,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 2 0.25 0.2 0.7 parallel_particles48_processes24_run1 24</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles72_processes24_run1</v>
@@ -1546,7 +2735,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 3 0.25 0.2 0.7 parallel_particles72_processes24_run1 24</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles96_processes24_run1</v>
@@ -1569,7 +2758,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 4 0.25 0.2 0.7 parallel_particles96_processes24_run1 24</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles120_processes24_run1</v>
@@ -1592,7 +2781,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 5 0.25 0.2 0.7 parallel_particles120_processes24_run1 24</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles48_processes48_run1</v>
@@ -1615,7 +2804,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 1 0.25 0.2 0.7 parallel_particles48_processes48_run1 48</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles96_processes48_run1</v>
@@ -1638,7 +2827,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 2 0.25 0.2 0.7 parallel_particles96_processes48_run1 48</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles144_processes48_run1</v>
@@ -1661,7 +2850,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 3 0.25 0.2 0.7 parallel_particles144_processes48_run1 48</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles192_processes48_run1</v>
@@ -1684,7 +2873,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 4 0.25 0.2 0.7 parallel_particles192_processes48_run1 48</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles240_processes48_run1</v>
@@ -1707,7 +2896,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 5 0.25 0.2 0.7 parallel_particles240_processes48_run1 48</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles96_processes96_run1</v>
@@ -1730,7 +2919,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 1 0.25 0.2 0.7 parallel_particles96_processes96_run1 96</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles192_processes96_run1</v>
@@ -1753,7 +2942,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 2 0.25 0.2 0.7 parallel_particles192_processes96_run1 96</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles288_processes96_run1</v>
@@ -1776,7 +2965,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 3 0.25 0.2 0.7 parallel_particles288_processes96_run1 96</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles384_processes96_run1</v>
@@ -1799,7 +2988,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 4 0.25 0.2 0.7 parallel_particles384_processes96_run1 96</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles480_processes96_run1</v>
@@ -1822,7 +3011,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 5 0.25 0.2 0.7 parallel_particles480_processes96_run1 96</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles12_processes12_run2</v>
@@ -1845,7 +3034,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 1 0.25 0.2 0.7 parallel_particles12_processes12_run2 12</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles24_processes12_run2</v>
@@ -1868,7 +3057,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 2 0.25 0.2 0.7 parallel_particles24_processes12_run2 12</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles36_processes12_run2</v>
@@ -1891,7 +3080,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 3 0.25 0.2 0.7 parallel_particles36_processes12_run2 12</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles48_processes12_run2</v>
@@ -1914,7 +3103,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 4 0.25 0.2 0.7 parallel_particles48_processes12_run2 12</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles60_processes12_run2</v>
@@ -1937,7 +3126,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 5 0.25 0.2 0.7 parallel_particles60_processes12_run2 12</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles1_processes1_run2</v>
@@ -1960,7 +3149,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 1 0.25 0.2 0.7 parallel_particles1_processes1_run2 1</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles2_processes1_run2</v>
@@ -1983,7 +3172,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 2 0.25 0.2 0.7 parallel_particles2_processes1_run2 1</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles3_processes1_run2</v>
@@ -2006,7 +3195,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 3 0.25 0.2 0.7 parallel_particles3_processes1_run2 1</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles4_processes1_run2</v>
@@ -2029,7 +3218,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 4 0.25 0.2 0.7 parallel_particles4_processes1_run2 1</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles5_processes1_run2</v>
@@ -2052,7 +3241,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 5 0.25 0.2 0.7 parallel_particles5_processes1_run2 1</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles24_processes24_run2</v>
@@ -2075,7 +3264,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 1 0.25 0.2 0.7 parallel_particles24_processes24_run2 24</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles48_processes24_run2</v>
@@ -2098,7 +3287,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 2 0.25 0.2 0.7 parallel_particles48_processes24_run2 24</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles72_processes24_run2</v>
@@ -2121,7 +3310,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 3 0.25 0.2 0.7 parallel_particles72_processes24_run2 24</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles96_processes24_run2</v>
@@ -2144,7 +3333,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 4 0.25 0.2 0.7 parallel_particles96_processes24_run2 24</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles120_processes24_run2</v>
@@ -2167,7 +3356,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 5 0.25 0.2 0.7 parallel_particles120_processes24_run2 24</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles48_processes48_run2</v>
@@ -2190,7 +3379,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 1 0.25 0.2 0.7 parallel_particles48_processes48_run2 48</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles96_processes48_run2</v>
@@ -2213,7 +3402,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 2 0.25 0.2 0.7 parallel_particles96_processes48_run2 48</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles144_processes48_run2</v>
@@ -2236,7 +3425,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 3 0.25 0.2 0.7 parallel_particles144_processes48_run2 48</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles192_processes48_run2</v>
@@ -2259,7 +3448,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 4 0.25 0.2 0.7 parallel_particles192_processes48_run2 48</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles240_processes48_run2</v>
@@ -2282,7 +3471,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 5 0.25 0.2 0.7 parallel_particles240_processes48_run2 48</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles96_processes96_run2</v>
@@ -2305,7 +3494,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 1 0.25 0.2 0.7 parallel_particles96_processes96_run2 96</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles192_processes96_run2</v>
@@ -2328,7 +3517,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 2 0.25 0.2 0.7 parallel_particles192_processes96_run2 96</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles288_processes96_run2</v>
@@ -2351,7 +3540,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 3 0.25 0.2 0.7 parallel_particles288_processes96_run2 96</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles384_processes96_run2</v>
@@ -2374,7 +3563,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 4 0.25 0.2 0.7 parallel_particles384_processes96_run2 96</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles480_processes96_run2</v>
@@ -2397,7 +3586,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 5 0.25 0.2 0.7 parallel_particles480_processes96_run2 96</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles12_processes12_run3</v>
@@ -2420,7 +3609,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 1 0.25 0.2 0.7 parallel_particles12_processes12_run3 12</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles24_processes12_run3</v>
@@ -2443,7 +3632,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 2 0.25 0.2 0.7 parallel_particles24_processes12_run3 12</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A75" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles36_processes12_run3</v>
@@ -2466,7 +3655,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 3 0.25 0.2 0.7 parallel_particles36_processes12_run3 12</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles48_processes12_run3</v>
@@ -2489,7 +3678,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 4 0.25 0.2 0.7 parallel_particles48_processes12_run3 12</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles60_processes12_run3</v>
@@ -2512,7 +3701,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 5 0.25 0.2 0.7 parallel_particles60_processes12_run3 12</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles1_processes1_run3</v>
@@ -2535,7 +3724,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 1 0.25 0.2 0.7 parallel_particles1_processes1_run3 1</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles2_processes1_run3</v>
@@ -2558,7 +3747,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 2 0.25 0.2 0.7 parallel_particles2_processes1_run3 1</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles3_processes1_run3</v>
@@ -2581,7 +3770,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 3 0.25 0.2 0.7 parallel_particles3_processes1_run3 1</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A81" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles4_processes1_run3</v>
@@ -2604,7 +3793,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 4 0.25 0.2 0.7 parallel_particles4_processes1_run3 1</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A82" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles5_processes1_run3</v>
@@ -2627,7 +3816,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 5 0.25 0.2 0.7 parallel_particles5_processes1_run3 1</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A83" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles24_processes24_run3</v>
@@ -2649,7 +3838,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 1 0.25 0.2 0.7 parallel_particles24_processes24_run3 24</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A84" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles48_processes24_run3</v>
@@ -2671,7 +3860,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 2 0.25 0.2 0.7 parallel_particles48_processes24_run3 24</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A85" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles72_processes24_run3</v>
@@ -2693,7 +3882,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 3 0.25 0.2 0.7 parallel_particles72_processes24_run3 24</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A86" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles96_processes24_run3</v>
@@ -2715,7 +3904,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 4 0.25 0.2 0.7 parallel_particles96_processes24_run3 24</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A87" s="8" t="str">
         <f t="shared" si="3"/>
         <v>parallel_particles120_processes24_run3</v>
@@ -2737,7 +3926,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 5 0.25 0.2 0.7 parallel_particles120_processes24_run3 24</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A88" s="8" t="str">
         <f t="shared" ref="A88:A97" si="5">"parallel_particles"&amp;B88*D88&amp;"_processes"&amp;D88&amp;"_run"&amp;E88</f>
         <v>parallel_particles48_processes48_run3</v>
@@ -2759,7 +3948,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 1 0.25 0.2 0.7 parallel_particles48_processes48_run3 48</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A89" s="8" t="str">
         <f t="shared" si="5"/>
         <v>parallel_particles96_processes48_run3</v>
@@ -2781,7 +3970,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 2 0.25 0.2 0.7 parallel_particles96_processes48_run3 48</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A90" s="8" t="str">
         <f t="shared" si="5"/>
         <v>parallel_particles144_processes48_run3</v>
@@ -2803,7 +3992,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 3 0.25 0.2 0.7 parallel_particles144_processes48_run3 48</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A91" s="8" t="str">
         <f t="shared" si="5"/>
         <v>parallel_particles192_processes48_run3</v>
@@ -2825,7 +4014,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 4 0.25 0.2 0.7 parallel_particles192_processes48_run3 48</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A92" s="8" t="str">
         <f t="shared" si="5"/>
         <v>parallel_particles240_processes48_run3</v>
@@ -2847,7 +4036,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 5 0.25 0.2 0.7 parallel_particles240_processes48_run3 48</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A93" s="8" t="str">
         <f t="shared" si="5"/>
         <v>parallel_particles96_processes96_run3</v>
@@ -2869,7 +4058,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 1 0.25 0.2 0.7 parallel_particles96_processes96_run3 96</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A94" s="8" t="str">
         <f t="shared" si="5"/>
         <v>parallel_particles192_processes96_run3</v>
@@ -2891,7 +4080,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 2 0.25 0.2 0.7 parallel_particles192_processes96_run3 96</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A95" s="8" t="str">
         <f t="shared" si="5"/>
         <v>parallel_particles288_processes96_run3</v>
@@ -2913,7 +4102,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 3 0.25 0.2 0.7 parallel_particles288_processes96_run3 96</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A96" s="8" t="str">
         <f t="shared" si="5"/>
         <v>parallel_particles384_processes96_run3</v>
@@ -2935,7 +4124,7 @@
         <v>srun python parallel_mpi_pso_algorithm.py "" 50 4 0.25 0.2 0.7 parallel_particles384_processes96_run3 96</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A97" s="8" t="str">
         <f t="shared" si="5"/>
         <v>parallel_particles480_processes96_run3</v>
@@ -2976,14 +4165,14 @@
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -2994,7 +4183,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>60</v>
       </c>
@@ -3006,7 +4195,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>60</v>
       </c>
@@ -3018,7 +4207,7 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>60</v>
       </c>
@@ -3030,7 +4219,7 @@
         <v>2160</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>60</v>
       </c>
@@ -3042,7 +4231,7 @@
         <v>2880</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>60</v>
       </c>
@@ -3054,7 +4243,7 @@
         <v>3600</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>20</v>
       </c>
@@ -3066,7 +4255,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>20</v>
       </c>
@@ -3078,7 +4267,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>20</v>
       </c>
@@ -3090,7 +4279,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>20</v>
       </c>
@@ -3102,7 +4291,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>20</v>
       </c>
@@ -3123,143 +4312,571 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04A4D4AE-7436-45D6-BD3C-D4B5923ED9C3}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13">
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="12">
         <v>48</v>
       </c>
-      <c r="B2" s="14">
-        <v>1</v>
-      </c>
-      <c r="C2" s="15">
+      <c r="B2" s="13">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14">
         <v>178.20760000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="13">
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="12">
         <v>48</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="13">
         <v>12</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="14">
         <v>20.2334</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="13">
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="12">
         <v>48</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>24</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="14">
         <v>13.4581</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="13">
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="12">
         <v>48</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="13">
         <v>48</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>10.029</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13">
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="12">
         <v>96</v>
       </c>
-      <c r="B6" s="14">
-        <v>1</v>
-      </c>
-      <c r="C6" s="15">
+      <c r="B6" s="13">
+        <v>1</v>
+      </c>
+      <c r="C6" s="14">
         <v>355.4391</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="13">
+    <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="12">
         <v>96</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="13">
         <v>24</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>20.783899999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="13">
+    <row r="8" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="12">
         <v>96</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="13">
         <v>48</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <v>13.7822</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="13">
+    <row r="9" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="12">
         <v>96</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="13">
         <v>96</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <v>10.606</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="15"/>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="13"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="15"/>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="13"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="15"/>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="15"/>
+    <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="15"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="17"/>
+    </row>
+    <row r="11" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+    </row>
+    <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="12"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="14"/>
+    </row>
+    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="12"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87F95DF-D073-43A4-A7F1-116A556B06B7}">
+  <dimension ref="A1:M19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.77734375" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>12</v>
+      </c>
+      <c r="B2" s="23">
+        <f>AVERAGE(C2:G2)</f>
+        <v>1.6308</v>
+      </c>
+      <c r="C2" s="22">
+        <v>2.2915000000000001</v>
+      </c>
+      <c r="D2" s="22">
+        <v>1.8355999999999999</v>
+      </c>
+      <c r="E2" s="22">
+        <v>1.2154</v>
+      </c>
+      <c r="F2" s="22">
+        <v>1.0092000000000001</v>
+      </c>
+      <c r="G2" s="22">
+        <v>1.8023</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>24</v>
+      </c>
+      <c r="B3" s="23">
+        <f t="shared" ref="B3:B8" si="0">AVERAGE(C3:G3)</f>
+        <v>1.2867799999999998</v>
+      </c>
+      <c r="C3" s="22">
+        <v>1.5331999999999999</v>
+      </c>
+      <c r="D3" s="22">
+        <v>1.7927</v>
+      </c>
+      <c r="E3" s="22">
+        <v>1.1651</v>
+      </c>
+      <c r="F3" s="22">
+        <v>0.99629999999999996</v>
+      </c>
+      <c r="G3" s="22">
+        <v>0.9466</v>
+      </c>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+    </row>
+    <row r="4" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>36</v>
+      </c>
+      <c r="B4" s="23">
+        <f t="shared" si="0"/>
+        <v>0.95776000000000006</v>
+      </c>
+      <c r="C4" s="22">
+        <v>0.89539999999999997</v>
+      </c>
+      <c r="D4" s="22">
+        <v>0.80989999999999995</v>
+      </c>
+      <c r="E4" s="22">
+        <v>1.052</v>
+      </c>
+      <c r="F4" s="22">
+        <v>1.0471999999999999</v>
+      </c>
+      <c r="G4" s="22">
+        <v>0.98429999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>72</v>
+      </c>
+      <c r="B5" s="23">
+        <f t="shared" si="0"/>
+        <v>0.87073999999999996</v>
+      </c>
+      <c r="C5" s="22">
+        <v>0.67549999999999999</v>
+      </c>
+      <c r="D5" s="22">
+        <v>0.9405</v>
+      </c>
+      <c r="E5" s="22">
+        <v>0.66200000000000003</v>
+      </c>
+      <c r="F5" s="22">
+        <v>0.86419999999999997</v>
+      </c>
+      <c r="G5" s="22">
+        <v>1.2115</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>144</v>
+      </c>
+      <c r="B6" s="23">
+        <f t="shared" si="0"/>
+        <v>0.75473999999999997</v>
+      </c>
+      <c r="C6" s="22">
+        <v>0.71220000000000006</v>
+      </c>
+      <c r="D6" s="22">
+        <v>0.72399999999999998</v>
+      </c>
+      <c r="E6" s="22">
+        <v>0.66920000000000002</v>
+      </c>
+      <c r="F6" s="22">
+        <v>0.86209999999999998</v>
+      </c>
+      <c r="G6" s="22">
+        <v>0.80620000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>288</v>
+      </c>
+      <c r="B7" s="23">
+        <f t="shared" si="0"/>
+        <v>0.71301999999999999</v>
+      </c>
+      <c r="C7" s="22">
+        <v>0.64080000000000004</v>
+      </c>
+      <c r="D7" s="22">
+        <v>0.68010000000000004</v>
+      </c>
+      <c r="E7" s="22">
+        <v>0.7319</v>
+      </c>
+      <c r="F7" s="22">
+        <v>0.71060000000000001</v>
+      </c>
+      <c r="G7" s="22">
+        <v>0.80169999999999997</v>
+      </c>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+    </row>
+    <row r="8" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>384</v>
+      </c>
+      <c r="B8" s="23">
+        <f t="shared" si="0"/>
+        <v>0.64498000000000011</v>
+      </c>
+      <c r="C8" s="22">
+        <v>0.67969999999999997</v>
+      </c>
+      <c r="D8" s="22">
+        <v>0.64270000000000005</v>
+      </c>
+      <c r="E8" s="22">
+        <v>0.64859999999999995</v>
+      </c>
+      <c r="F8" s="22">
+        <v>0.62719999999999998</v>
+      </c>
+      <c r="G8" s="22">
+        <v>0.62670000000000003</v>
+      </c>
+      <c r="I8" s="20"/>
+    </row>
+    <row r="9" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C9" s="21"/>
+      <c r="I9" s="21"/>
+    </row>
+    <row r="10" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>12</v>
+      </c>
+      <c r="B11" s="23">
+        <f t="shared" ref="B11:B17" si="1">AVERAGE(C11:G11)</f>
+        <v>3.2825200000000003</v>
+      </c>
+      <c r="C11" s="22">
+        <v>4.5621999999999998</v>
+      </c>
+      <c r="D11" s="22">
+        <v>3.1238999999999999</v>
+      </c>
+      <c r="E11" s="22">
+        <v>3.1331000000000002</v>
+      </c>
+      <c r="F11" s="22">
+        <v>2.6568000000000001</v>
+      </c>
+      <c r="G11" s="22">
+        <v>2.9365999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>24</v>
+      </c>
+      <c r="B12" s="23">
+        <f t="shared" si="1"/>
+        <v>3.2276600000000002</v>
+      </c>
+      <c r="C12" s="22">
+        <v>3.0581</v>
+      </c>
+      <c r="D12" s="22">
+        <v>2.899</v>
+      </c>
+      <c r="E12" s="22">
+        <v>2.7231000000000001</v>
+      </c>
+      <c r="F12" s="22">
+        <v>4.5505000000000004</v>
+      </c>
+      <c r="G12" s="22">
+        <v>2.9076</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>36</v>
+      </c>
+      <c r="B13" s="23">
+        <f t="shared" si="1"/>
+        <v>2.4554</v>
+      </c>
+      <c r="C13" s="22">
+        <v>2.3189000000000002</v>
+      </c>
+      <c r="D13" s="22">
+        <v>2.5550000000000002</v>
+      </c>
+      <c r="E13" s="22">
+        <v>1.9999</v>
+      </c>
+      <c r="F13" s="22">
+        <v>3.0747</v>
+      </c>
+      <c r="G13" s="22">
+        <v>2.3285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>72</v>
+      </c>
+      <c r="B14" s="23">
+        <f t="shared" si="1"/>
+        <v>2.1260000000000003</v>
+      </c>
+      <c r="C14" s="22">
+        <v>2.0024999999999999</v>
+      </c>
+      <c r="D14" s="22">
+        <v>1.9390000000000001</v>
+      </c>
+      <c r="E14" s="22">
+        <v>2.4798</v>
+      </c>
+      <c r="F14" s="22">
+        <v>2.0282</v>
+      </c>
+      <c r="G14" s="22">
+        <v>2.1804999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>144</v>
+      </c>
+      <c r="B15" s="23">
+        <f t="shared" si="1"/>
+        <v>1.8787200000000002</v>
+      </c>
+      <c r="C15" s="22">
+        <v>1.9444999999999999</v>
+      </c>
+      <c r="D15" s="22">
+        <v>1.9233</v>
+      </c>
+      <c r="E15" s="22">
+        <v>1.8596999999999999</v>
+      </c>
+      <c r="F15" s="22">
+        <v>1.8515999999999999</v>
+      </c>
+      <c r="G15" s="22">
+        <v>1.8145</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>288</v>
+      </c>
+      <c r="B16" s="23">
+        <f t="shared" si="1"/>
+        <v>1.8597600000000001</v>
+      </c>
+      <c r="C16" s="22">
+        <v>1.7903</v>
+      </c>
+      <c r="D16" s="22">
+        <v>1.7709999999999999</v>
+      </c>
+      <c r="E16" s="22">
+        <v>2.0419</v>
+      </c>
+      <c r="F16" s="22">
+        <v>1.8248</v>
+      </c>
+      <c r="G16" s="22">
+        <v>1.8708</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>384</v>
+      </c>
+      <c r="B17" s="23">
+        <f t="shared" si="1"/>
+        <v>1.7406399999999997</v>
+      </c>
+      <c r="C17" s="22">
+        <v>1.6684000000000001</v>
+      </c>
+      <c r="D17" s="22">
+        <v>1.7325999999999999</v>
+      </c>
+      <c r="E17" s="22">
+        <v>1.7713000000000001</v>
+      </c>
+      <c r="F17" s="22">
+        <v>1.8209</v>
+      </c>
+      <c r="G17" s="22">
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C18" s="24"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+    </row>
+    <row r="19" spans="1:7" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="C19" s="21"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>